<commit_message>
update to 2024 crop data
</commit_message>
<xml_diff>
--- a/analytics/modified_data/tbf_market_garden_data_2024_clean.xlsx
+++ b/analytics/modified_data/tbf_market_garden_data_2024_clean.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="490" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="618" uniqueCount="219">
   <si>
     <t>crop</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>2024-03-22</t>
+  </si>
+  <si>
+    <t>2024-04-04</t>
   </si>
   <si>
     <t>sow_fert_type_npk_1</t>
@@ -765,469 +768,469 @@
         <v>58</v>
       </c>
       <c r="P1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="R1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="T1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="U1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="V1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="W1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="X1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Y1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AC1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AD1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AE1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AF1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AG1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AH1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AI1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AJ1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AK1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AL1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AM1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AN1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AO1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AP1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AQ1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AR1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AS1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AT1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AU1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AV1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AW1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AX1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AY1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AZ1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="BA1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="BB1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="BC1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BD1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="BE1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="BF1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="BG1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="BH1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="BI1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="BJ1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="BK1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="BL1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="BM1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="BN1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="BO1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="BP1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="BQ1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="BR1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="BS1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="BT1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="BU1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="BV1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="BW1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="BX1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="BY1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BZ1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CA1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="CB1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="CC1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CD1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="CE1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="CF1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="CG1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="CH1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="CI1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="CJ1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="CK1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="CL1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="CM1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CN1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CO1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CP1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CQ1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="CR1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CS1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CT1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CW1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="CX1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="CY1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="CZ1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DA1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="DB1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="DC1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="DD1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="DE1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="DF1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="DG1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="DH1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="DI1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="DJ1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="DK1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="DL1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="DM1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="DN1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="DO1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="DP1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="DQ1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="DR1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="DS1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="DT1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="DU1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="DV1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="DW1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="DX1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="DY1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="DZ1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="EA1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="EB1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="EC1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="ED1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="EE1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="EF1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="EG1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="EH1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="EI1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="EJ1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="EK1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="EL1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="EM1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="EN1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="EO1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="EP1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="EQ1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="ER1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="ES1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="ET1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="EU1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="EV1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="EW1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="EX1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="EY1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="EZ1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="FA1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="FB1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="FC1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="FD1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="FE1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="FF1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="FG1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="FH1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="FI1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="FJ1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="FK1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="FL1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="FM1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="FN1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2">
@@ -1275,10 +1278,18 @@
       <c r="R2" t="s">
         <v>51</v>
       </c>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
+      <c r="S2" t="s">
+        <v>51</v>
+      </c>
+      <c r="T2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" t="s">
+        <v>51</v>
+      </c>
+      <c r="V2" t="s">
+        <v>51</v>
+      </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -1471,18 +1482,26 @@
         <v>59</v>
       </c>
       <c r="P3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R3" t="s">
-        <v>65</v>
-      </c>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S3" t="s">
+        <v>60</v>
+      </c>
+      <c r="T3" t="s">
+        <v>62</v>
+      </c>
+      <c r="U3" t="s">
+        <v>64</v>
+      </c>
+      <c r="V3" t="s">
+        <v>66</v>
+      </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
@@ -1675,18 +1694,26 @@
         <v>59</v>
       </c>
       <c r="P4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R4" t="s">
-        <v>65</v>
-      </c>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S4" t="s">
+        <v>60</v>
+      </c>
+      <c r="T4" t="s">
+        <v>62</v>
+      </c>
+      <c r="U4" t="s">
+        <v>64</v>
+      </c>
+      <c r="V4" t="s">
+        <v>66</v>
+      </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
@@ -1879,18 +1906,26 @@
         <v>59</v>
       </c>
       <c r="P5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R5" t="s">
-        <v>65</v>
-      </c>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S5" t="s">
+        <v>60</v>
+      </c>
+      <c r="T5" t="s">
+        <v>62</v>
+      </c>
+      <c r="U5" t="s">
+        <v>64</v>
+      </c>
+      <c r="V5" t="s">
+        <v>66</v>
+      </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
@@ -2083,18 +2118,26 @@
         <v>59</v>
       </c>
       <c r="P6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R6" t="s">
-        <v>65</v>
-      </c>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S6" t="s">
+        <v>60</v>
+      </c>
+      <c r="T6" t="s">
+        <v>62</v>
+      </c>
+      <c r="U6" t="s">
+        <v>64</v>
+      </c>
+      <c r="V6" t="s">
+        <v>66</v>
+      </c>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
@@ -2287,18 +2330,26 @@
         <v>59</v>
       </c>
       <c r="P7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R7" t="s">
-        <v>65</v>
-      </c>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S7" t="s">
+        <v>60</v>
+      </c>
+      <c r="T7" t="s">
+        <v>62</v>
+      </c>
+      <c r="U7" t="s">
+        <v>64</v>
+      </c>
+      <c r="V7" t="s">
+        <v>66</v>
+      </c>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
@@ -2491,18 +2542,26 @@
         <v>59</v>
       </c>
       <c r="P8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R8" t="s">
-        <v>65</v>
-      </c>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S8" t="s">
+        <v>60</v>
+      </c>
+      <c r="T8" t="s">
+        <v>62</v>
+      </c>
+      <c r="U8" t="s">
+        <v>64</v>
+      </c>
+      <c r="V8" t="s">
+        <v>66</v>
+      </c>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
@@ -2697,18 +2756,26 @@
         <v>59</v>
       </c>
       <c r="P9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R9" t="s">
-        <v>65</v>
-      </c>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S9" t="s">
+        <v>60</v>
+      </c>
+      <c r="T9" t="s">
+        <v>62</v>
+      </c>
+      <c r="U9" t="s">
+        <v>64</v>
+      </c>
+      <c r="V9" t="s">
+        <v>66</v>
+      </c>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
@@ -2903,18 +2970,26 @@
         <v>59</v>
       </c>
       <c r="P10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R10" t="s">
-        <v>65</v>
-      </c>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S10" t="s">
+        <v>60</v>
+      </c>
+      <c r="T10" t="s">
+        <v>62</v>
+      </c>
+      <c r="U10" t="s">
+        <v>64</v>
+      </c>
+      <c r="V10" t="s">
+        <v>66</v>
+      </c>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
@@ -3109,18 +3184,26 @@
         <v>59</v>
       </c>
       <c r="P11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R11" t="s">
-        <v>65</v>
-      </c>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S11" t="s">
+        <v>60</v>
+      </c>
+      <c r="T11" t="s">
+        <v>62</v>
+      </c>
+      <c r="U11" t="s">
+        <v>64</v>
+      </c>
+      <c r="V11" t="s">
+        <v>66</v>
+      </c>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
@@ -3315,18 +3398,26 @@
         <v>59</v>
       </c>
       <c r="P12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R12" t="s">
-        <v>65</v>
-      </c>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S12" t="s">
+        <v>60</v>
+      </c>
+      <c r="T12" t="s">
+        <v>62</v>
+      </c>
+      <c r="U12" t="s">
+        <v>64</v>
+      </c>
+      <c r="V12" t="s">
+        <v>66</v>
+      </c>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
@@ -3521,18 +3612,26 @@
         <v>59</v>
       </c>
       <c r="P13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R13" t="s">
-        <v>65</v>
-      </c>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S13" t="s">
+        <v>60</v>
+      </c>
+      <c r="T13" t="s">
+        <v>62</v>
+      </c>
+      <c r="U13" t="s">
+        <v>64</v>
+      </c>
+      <c r="V13" t="s">
+        <v>66</v>
+      </c>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
@@ -3727,18 +3826,26 @@
         <v>59</v>
       </c>
       <c r="P14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R14" t="s">
-        <v>65</v>
-      </c>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S14" t="s">
+        <v>60</v>
+      </c>
+      <c r="T14" t="s">
+        <v>62</v>
+      </c>
+      <c r="U14" t="s">
+        <v>64</v>
+      </c>
+      <c r="V14" t="s">
+        <v>66</v>
+      </c>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
@@ -3933,18 +4040,26 @@
         <v>59</v>
       </c>
       <c r="P15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R15" t="s">
-        <v>65</v>
-      </c>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S15" t="s">
+        <v>60</v>
+      </c>
+      <c r="T15" t="s">
+        <v>62</v>
+      </c>
+      <c r="U15" t="s">
+        <v>64</v>
+      </c>
+      <c r="V15" t="s">
+        <v>66</v>
+      </c>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
@@ -4139,18 +4254,26 @@
         <v>59</v>
       </c>
       <c r="P16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R16" t="s">
-        <v>65</v>
-      </c>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S16" t="s">
+        <v>60</v>
+      </c>
+      <c r="T16" t="s">
+        <v>62</v>
+      </c>
+      <c r="U16" t="s">
+        <v>64</v>
+      </c>
+      <c r="V16" t="s">
+        <v>66</v>
+      </c>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
@@ -4345,18 +4468,26 @@
         <v>59</v>
       </c>
       <c r="P17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R17" t="s">
-        <v>65</v>
-      </c>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S17" t="s">
+        <v>60</v>
+      </c>
+      <c r="T17" t="s">
+        <v>62</v>
+      </c>
+      <c r="U17" t="s">
+        <v>64</v>
+      </c>
+      <c r="V17" t="s">
+        <v>66</v>
+      </c>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
@@ -4551,18 +4682,26 @@
         <v>59</v>
       </c>
       <c r="P18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R18" t="s">
-        <v>65</v>
-      </c>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S18" t="s">
+        <v>60</v>
+      </c>
+      <c r="T18" t="s">
+        <v>62</v>
+      </c>
+      <c r="U18" t="s">
+        <v>64</v>
+      </c>
+      <c r="V18" t="s">
+        <v>66</v>
+      </c>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
@@ -4757,18 +4896,26 @@
         <v>59</v>
       </c>
       <c r="P19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R19" t="s">
-        <v>65</v>
-      </c>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S19" t="s">
+        <v>60</v>
+      </c>
+      <c r="T19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U19" t="s">
+        <v>64</v>
+      </c>
+      <c r="V19" t="s">
+        <v>66</v>
+      </c>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
@@ -4963,18 +5110,26 @@
         <v>59</v>
       </c>
       <c r="P20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R20" t="s">
-        <v>65</v>
-      </c>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="S20" t="s">
+        <v>60</v>
+      </c>
+      <c r="T20" t="s">
+        <v>62</v>
+      </c>
+      <c r="U20" t="s">
+        <v>64</v>
+      </c>
+      <c r="V20" t="s">
+        <v>66</v>
+      </c>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
@@ -5166,21 +5321,29 @@
         <v>57</v>
       </c>
       <c r="O21" t="s">
+        <v>60</v>
+      </c>
+      <c r="P21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>64</v>
+      </c>
+      <c r="R21" t="s">
+        <v>66</v>
+      </c>
+      <c r="S21" t="s">
         <v>51</v>
       </c>
-      <c r="P21" t="s">
+      <c r="T21" t="s">
         <v>51</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="U21" t="s">
         <v>51</v>
       </c>
-      <c r="R21" t="s">
+      <c r="V21" t="s">
         <v>51</v>
       </c>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
@@ -5372,21 +5535,29 @@
         <v>57</v>
       </c>
       <c r="O22" t="s">
+        <v>60</v>
+      </c>
+      <c r="P22" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>64</v>
+      </c>
+      <c r="R22" t="s">
+        <v>66</v>
+      </c>
+      <c r="S22" t="s">
         <v>51</v>
       </c>
-      <c r="P22" t="s">
+      <c r="T22" t="s">
         <v>51</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="U22" t="s">
         <v>51</v>
       </c>
-      <c r="R22" t="s">
+      <c r="V22" t="s">
         <v>51</v>
       </c>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
@@ -5578,21 +5749,29 @@
         <v>57</v>
       </c>
       <c r="O23" t="s">
+        <v>60</v>
+      </c>
+      <c r="P23" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>64</v>
+      </c>
+      <c r="R23" t="s">
+        <v>66</v>
+      </c>
+      <c r="S23" t="s">
         <v>51</v>
       </c>
-      <c r="P23" t="s">
+      <c r="T23" t="s">
         <v>51</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="U23" t="s">
         <v>51</v>
       </c>
-      <c r="R23" t="s">
+      <c r="V23" t="s">
         <v>51</v>
       </c>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
@@ -5784,21 +5963,29 @@
         <v>57</v>
       </c>
       <c r="O24" t="s">
+        <v>60</v>
+      </c>
+      <c r="P24" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>64</v>
+      </c>
+      <c r="R24" t="s">
+        <v>66</v>
+      </c>
+      <c r="S24" t="s">
         <v>51</v>
       </c>
-      <c r="P24" t="s">
+      <c r="T24" t="s">
         <v>51</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="U24" t="s">
         <v>51</v>
       </c>
-      <c r="R24" t="s">
+      <c r="V24" t="s">
         <v>51</v>
       </c>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
@@ -5990,21 +6177,29 @@
         <v>57</v>
       </c>
       <c r="O25" t="s">
+        <v>60</v>
+      </c>
+      <c r="P25" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>64</v>
+      </c>
+      <c r="R25" t="s">
+        <v>66</v>
+      </c>
+      <c r="S25" t="s">
         <v>51</v>
       </c>
-      <c r="P25" t="s">
+      <c r="T25" t="s">
         <v>51</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="U25" t="s">
         <v>51</v>
       </c>
-      <c r="R25" t="s">
+      <c r="V25" t="s">
         <v>51</v>
       </c>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>
@@ -6196,21 +6391,29 @@
         <v>57</v>
       </c>
       <c r="O26" t="s">
+        <v>60</v>
+      </c>
+      <c r="P26" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>64</v>
+      </c>
+      <c r="R26" t="s">
+        <v>66</v>
+      </c>
+      <c r="S26" t="s">
         <v>51</v>
       </c>
-      <c r="P26" t="s">
+      <c r="T26" t="s">
         <v>51</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="U26" t="s">
         <v>51</v>
       </c>
-      <c r="R26" t="s">
+      <c r="V26" t="s">
         <v>51</v>
       </c>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
@@ -6398,21 +6601,29 @@
         <v>57</v>
       </c>
       <c r="O27" t="s">
+        <v>60</v>
+      </c>
+      <c r="P27" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>64</v>
+      </c>
+      <c r="R27" t="s">
+        <v>66</v>
+      </c>
+      <c r="S27" t="s">
         <v>51</v>
       </c>
-      <c r="P27" t="s">
+      <c r="T27" t="s">
         <v>51</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="U27" t="s">
         <v>51</v>
       </c>
-      <c r="R27" t="s">
+      <c r="V27" t="s">
         <v>51</v>
       </c>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
       <c r="Y27" s="1"/>
@@ -6604,21 +6815,29 @@
         <v>57</v>
       </c>
       <c r="O28" t="s">
+        <v>60</v>
+      </c>
+      <c r="P28" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>64</v>
+      </c>
+      <c r="R28" t="s">
+        <v>66</v>
+      </c>
+      <c r="S28" t="s">
         <v>51</v>
       </c>
-      <c r="P28" t="s">
+      <c r="T28" t="s">
         <v>51</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="U28" t="s">
         <v>51</v>
       </c>
-      <c r="R28" t="s">
+      <c r="V28" t="s">
         <v>51</v>
       </c>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
       <c r="Y28" s="1"/>
@@ -6810,21 +7029,29 @@
         <v>57</v>
       </c>
       <c r="O29" t="s">
+        <v>60</v>
+      </c>
+      <c r="P29" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>64</v>
+      </c>
+      <c r="R29" t="s">
+        <v>66</v>
+      </c>
+      <c r="S29" t="s">
         <v>51</v>
       </c>
-      <c r="P29" t="s">
+      <c r="T29" t="s">
         <v>51</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="U29" t="s">
         <v>51</v>
       </c>
-      <c r="R29" t="s">
+      <c r="V29" t="s">
         <v>51</v>
       </c>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
@@ -7016,21 +7243,29 @@
         <v>57</v>
       </c>
       <c r="O30" t="s">
+        <v>60</v>
+      </c>
+      <c r="P30" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>64</v>
+      </c>
+      <c r="R30" t="s">
+        <v>66</v>
+      </c>
+      <c r="S30" t="s">
         <v>51</v>
       </c>
-      <c r="P30" t="s">
+      <c r="T30" t="s">
         <v>51</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="U30" t="s">
         <v>51</v>
       </c>
-      <c r="R30" t="s">
+      <c r="V30" t="s">
         <v>51</v>
       </c>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
       <c r="Y30" s="1"/>
@@ -7222,21 +7457,29 @@
         <v>57</v>
       </c>
       <c r="O31" t="s">
+        <v>60</v>
+      </c>
+      <c r="P31" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>64</v>
+      </c>
+      <c r="R31" t="s">
+        <v>66</v>
+      </c>
+      <c r="S31" t="s">
         <v>51</v>
       </c>
-      <c r="P31" t="s">
+      <c r="T31" t="s">
         <v>51</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="U31" t="s">
         <v>51</v>
       </c>
-      <c r="R31" t="s">
+      <c r="V31" t="s">
         <v>51</v>
       </c>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
@@ -7428,21 +7671,29 @@
         <v>57</v>
       </c>
       <c r="O32" t="s">
+        <v>60</v>
+      </c>
+      <c r="P32" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>64</v>
+      </c>
+      <c r="R32" t="s">
+        <v>66</v>
+      </c>
+      <c r="S32" t="s">
         <v>51</v>
       </c>
-      <c r="P32" t="s">
+      <c r="T32" t="s">
         <v>51</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="U32" t="s">
         <v>51</v>
       </c>
-      <c r="R32" t="s">
+      <c r="V32" t="s">
         <v>51</v>
       </c>
-      <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
-      <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
@@ -7634,21 +7885,29 @@
         <v>57</v>
       </c>
       <c r="O33" t="s">
+        <v>60</v>
+      </c>
+      <c r="P33" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>64</v>
+      </c>
+      <c r="R33" t="s">
+        <v>66</v>
+      </c>
+      <c r="S33" t="s">
         <v>51</v>
       </c>
-      <c r="P33" t="s">
+      <c r="T33" t="s">
         <v>51</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="U33" t="s">
         <v>51</v>
       </c>
-      <c r="R33" t="s">
+      <c r="V33" t="s">
         <v>51</v>
       </c>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
       <c r="Y33" s="1"/>

</xml_diff>

<commit_message>
updates to 2024 crop data
</commit_message>
<xml_diff>
--- a/analytics/modified_data/tbf_market_garden_data_2024_clean.xlsx
+++ b/analytics/modified_data/tbf_market_garden_data_2024_clean.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="618" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="778" uniqueCount="225">
   <si>
     <t>crop</t>
   </si>
@@ -192,6 +192,9 @@
     <t>sow_fert_date_1</t>
   </si>
   <si>
+    <t>2024-04-09</t>
+  </si>
+  <si>
     <t>2024-03-22</t>
   </si>
   <si>
@@ -201,24 +204,36 @@
     <t>sow_fert_type_npk_1</t>
   </si>
   <si>
+    <t>3-4-4</t>
+  </si>
+  <si>
     <t>2-2-2</t>
   </si>
   <si>
     <t>sow_fert_type_name_1</t>
   </si>
   <si>
+    <t>Espoma- Garden-tone</t>
+  </si>
+  <si>
     <t>Espoma- Organic Grow!</t>
   </si>
   <si>
     <t>sow_fert_dose_1</t>
   </si>
   <si>
+    <t>na</t>
+  </si>
+  <si>
     <t>half</t>
   </si>
   <si>
     <t>sow_fert_date_2</t>
   </si>
   <si>
+    <t>2024-04-15</t>
+  </si>
+  <si>
     <t>sow_fert_type_npk_2</t>
   </si>
   <si>
@@ -259,6 +274,9 @@
   </si>
   <si>
     <t>transp_date_1</t>
+  </si>
+  <si>
+    <t>2024-04-13</t>
   </si>
   <si>
     <t>transp_med_1</t>
@@ -768,469 +786,469 @@
         <v>58</v>
       </c>
       <c r="P1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="S1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="T1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="U1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="V1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="W1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="X1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="Y1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="Z1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="AA1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="AB1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="AC1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="AD1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="AE1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="AF1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="AG1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="AH1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="AI1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="AJ1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="AK1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="AL1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="AM1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="AN1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="AO1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="AP1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="AQ1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="AR1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="AS1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="AT1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="AU1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="AV1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="AW1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="AX1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="AY1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="AZ1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="BA1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="BB1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="BC1" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="BD1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="BE1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="BF1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="BG1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="BH1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="BI1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="BJ1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="BK1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="BL1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="BM1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="BN1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="BO1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="BP1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="BQ1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="BR1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="BS1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="BT1" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="BU1" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="BV1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="BW1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="BX1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="BY1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="BZ1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="CA1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="CB1" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="CC1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="CD1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="CE1" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="CF1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="CG1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="CH1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="CI1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="CJ1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="CK1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="CL1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="CM1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="CN1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="CO1" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="CP1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="CQ1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="CR1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="CS1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="CT1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="CU1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="CV1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="CW1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="CX1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="CY1" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="CZ1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="DA1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="DB1" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="DC1" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="DD1" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="DE1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="DF1" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="DG1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="DH1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="DI1" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="DJ1" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="DK1" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="DL1" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="DM1" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="DN1" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="DO1" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="DP1" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="DQ1" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="DR1" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="DS1" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="DT1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="DU1" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="DV1" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="DW1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="DX1" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="DY1" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="DZ1" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="EA1" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="EB1" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="EC1" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="ED1" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="EE1" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="EF1" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="EG1" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="EH1" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="EI1" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="EJ1" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="EK1" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="EL1" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="EM1" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="EN1" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="EO1" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="EP1" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="EQ1" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="ER1" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="ES1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="ET1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="EU1" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="EV1" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="EW1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="EX1" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="EY1" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="EZ1" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="FA1" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="FB1" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="FC1" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="FD1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="FE1" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="FF1" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="FG1" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="FH1" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="FI1" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="FJ1" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="FK1" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="FL1" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="FM1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="FN1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2">
@@ -1257,7 +1275,9 @@
       <c r="I2" s="1">
         <v>18</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1">
+        <v>18</v>
+      </c>
       <c r="K2" t="s">
         <v>51</v>
       </c>
@@ -1267,16 +1287,16 @@
         <v>51</v>
       </c>
       <c r="O2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="P2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="Q2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="R2" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="S2" t="s">
         <v>51</v>
@@ -1290,17 +1310,27 @@
       <c r="V2" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
+      <c r="W2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>51</v>
+      </c>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
+      <c r="AG2" t="s">
+        <v>51</v>
+      </c>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
@@ -1467,7 +1497,9 @@
       <c r="I3" s="1">
         <v>3</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1">
+        <v>2</v>
+      </c>
       <c r="K3" t="s">
         <v>52</v>
       </c>
@@ -1479,42 +1511,56 @@
         <v>57</v>
       </c>
       <c r="O3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q3" t="s">
+        <v>67</v>
+      </c>
+      <c r="R3" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" t="s">
         <v>64</v>
       </c>
-      <c r="R3" t="s">
-        <v>66</v>
-      </c>
-      <c r="S3" t="s">
-        <v>60</v>
-      </c>
-      <c r="T3" t="s">
-        <v>62</v>
-      </c>
       <c r="U3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="V3" t="s">
-        <v>66</v>
-      </c>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W3" t="s">
+        <v>51</v>
+      </c>
+      <c r="X3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>51</v>
+      </c>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
+      <c r="AG3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>8</v>
+      </c>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
@@ -1679,7 +1725,9 @@
       <c r="I4" s="1">
         <v>3</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
       <c r="K4" t="s">
         <v>52</v>
       </c>
@@ -1691,42 +1739,56 @@
         <v>57</v>
       </c>
       <c r="O4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R4" t="s">
+        <v>70</v>
+      </c>
+      <c r="S4" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" t="s">
         <v>64</v>
       </c>
-      <c r="R4" t="s">
-        <v>66</v>
-      </c>
-      <c r="S4" t="s">
-        <v>60</v>
-      </c>
-      <c r="T4" t="s">
-        <v>62</v>
-      </c>
       <c r="U4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="V4" t="s">
-        <v>66</v>
-      </c>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W4" t="s">
+        <v>51</v>
+      </c>
+      <c r="X4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>51</v>
+      </c>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
+      <c r="AG4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>1</v>
+      </c>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
@@ -1891,7 +1953,9 @@
       <c r="I5" s="1">
         <v>4</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1">
+        <v>2</v>
+      </c>
       <c r="K5" t="s">
         <v>52</v>
       </c>
@@ -1903,42 +1967,56 @@
         <v>57</v>
       </c>
       <c r="O5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q5" t="s">
+        <v>67</v>
+      </c>
+      <c r="R5" t="s">
+        <v>70</v>
+      </c>
+      <c r="S5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T5" t="s">
         <v>64</v>
       </c>
-      <c r="R5" t="s">
-        <v>66</v>
-      </c>
-      <c r="S5" t="s">
-        <v>60</v>
-      </c>
-      <c r="T5" t="s">
-        <v>62</v>
-      </c>
       <c r="U5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="V5" t="s">
-        <v>66</v>
-      </c>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W5" t="s">
+        <v>51</v>
+      </c>
+      <c r="X5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>51</v>
+      </c>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
+      <c r="AG5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="AI5" s="1">
+        <v>19</v>
+      </c>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1"/>
@@ -2103,7 +2181,9 @@
       <c r="I6" s="1">
         <v>4</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1">
+        <v>2</v>
+      </c>
       <c r="K6" t="s">
         <v>52</v>
       </c>
@@ -2115,42 +2195,56 @@
         <v>57</v>
       </c>
       <c r="O6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q6" t="s">
+        <v>67</v>
+      </c>
+      <c r="R6" t="s">
+        <v>70</v>
+      </c>
+      <c r="S6" t="s">
+        <v>61</v>
+      </c>
+      <c r="T6" t="s">
         <v>64</v>
       </c>
-      <c r="R6" t="s">
-        <v>66</v>
-      </c>
-      <c r="S6" t="s">
-        <v>60</v>
-      </c>
-      <c r="T6" t="s">
-        <v>62</v>
-      </c>
       <c r="U6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="V6" t="s">
-        <v>66</v>
-      </c>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W6" t="s">
+        <v>51</v>
+      </c>
+      <c r="X6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>51</v>
+      </c>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
+      <c r="AG6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>18</v>
+      </c>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AL6" s="1"/>
@@ -2315,7 +2409,9 @@
       <c r="I7" s="1">
         <v>4</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1">
+        <v>2</v>
+      </c>
       <c r="K7" t="s">
         <v>52</v>
       </c>
@@ -2327,42 +2423,56 @@
         <v>57</v>
       </c>
       <c r="O7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q7" t="s">
+        <v>67</v>
+      </c>
+      <c r="R7" t="s">
+        <v>70</v>
+      </c>
+      <c r="S7" t="s">
+        <v>61</v>
+      </c>
+      <c r="T7" t="s">
         <v>64</v>
       </c>
-      <c r="R7" t="s">
-        <v>66</v>
-      </c>
-      <c r="S7" t="s">
-        <v>60</v>
-      </c>
-      <c r="T7" t="s">
-        <v>62</v>
-      </c>
       <c r="U7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="V7" t="s">
-        <v>66</v>
-      </c>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W7" t="s">
+        <v>51</v>
+      </c>
+      <c r="X7" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>51</v>
+      </c>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
-      <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
-      <c r="AI7" s="1"/>
+      <c r="AG7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="AI7" s="1">
+        <v>20</v>
+      </c>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
       <c r="AL7" s="1"/>
@@ -2527,7 +2637,9 @@
       <c r="I8" s="1">
         <v>4</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1">
+        <v>2</v>
+      </c>
       <c r="K8" t="s">
         <v>52</v>
       </c>
@@ -2539,42 +2651,56 @@
         <v>57</v>
       </c>
       <c r="O8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q8" t="s">
+        <v>67</v>
+      </c>
+      <c r="R8" t="s">
+        <v>70</v>
+      </c>
+      <c r="S8" t="s">
+        <v>61</v>
+      </c>
+      <c r="T8" t="s">
         <v>64</v>
       </c>
-      <c r="R8" t="s">
-        <v>66</v>
-      </c>
-      <c r="S8" t="s">
-        <v>60</v>
-      </c>
-      <c r="T8" t="s">
-        <v>62</v>
-      </c>
       <c r="U8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="V8" t="s">
-        <v>66</v>
-      </c>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W8" t="s">
+        <v>51</v>
+      </c>
+      <c r="X8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>51</v>
+      </c>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
-      <c r="AG8" s="1"/>
-      <c r="AH8" s="1"/>
-      <c r="AI8" s="1"/>
+      <c r="AG8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="AI8" s="1">
+        <v>20</v>
+      </c>
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1"/>
       <c r="AL8" s="1"/>
@@ -2739,7 +2865,9 @@
       <c r="I9" s="1">
         <v>4</v>
       </c>
-      <c r="J9" s="1"/>
+      <c r="J9" s="1">
+        <v>3</v>
+      </c>
       <c r="K9" t="s">
         <v>53</v>
       </c>
@@ -2753,40 +2881,50 @@
         <v>57</v>
       </c>
       <c r="O9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q9" t="s">
+        <v>67</v>
+      </c>
+      <c r="R9" t="s">
+        <v>70</v>
+      </c>
+      <c r="S9" t="s">
+        <v>61</v>
+      </c>
+      <c r="T9" t="s">
         <v>64</v>
       </c>
-      <c r="R9" t="s">
-        <v>66</v>
-      </c>
-      <c r="S9" t="s">
-        <v>60</v>
-      </c>
-      <c r="T9" t="s">
-        <v>62</v>
-      </c>
       <c r="U9" t="s">
+        <v>67</v>
+      </c>
+      <c r="V9" t="s">
+        <v>70</v>
+      </c>
+      <c r="W9" t="s">
+        <v>72</v>
+      </c>
+      <c r="X9" t="s">
         <v>64</v>
       </c>
-      <c r="V9" t="s">
-        <v>66</v>
-      </c>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
+      <c r="Y9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>70</v>
+      </c>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
+      <c r="AG9" t="s">
+        <v>51</v>
+      </c>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
@@ -2953,7 +3091,9 @@
       <c r="I10" s="1">
         <v>3</v>
       </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1">
+        <v>3</v>
+      </c>
       <c r="K10" t="s">
         <v>53</v>
       </c>
@@ -2967,40 +3107,50 @@
         <v>57</v>
       </c>
       <c r="O10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q10" t="s">
+        <v>67</v>
+      </c>
+      <c r="R10" t="s">
+        <v>70</v>
+      </c>
+      <c r="S10" t="s">
+        <v>61</v>
+      </c>
+      <c r="T10" t="s">
         <v>64</v>
       </c>
-      <c r="R10" t="s">
-        <v>66</v>
-      </c>
-      <c r="S10" t="s">
-        <v>60</v>
-      </c>
-      <c r="T10" t="s">
-        <v>62</v>
-      </c>
       <c r="U10" t="s">
+        <v>67</v>
+      </c>
+      <c r="V10" t="s">
+        <v>70</v>
+      </c>
+      <c r="W10" t="s">
+        <v>72</v>
+      </c>
+      <c r="X10" t="s">
         <v>64</v>
       </c>
-      <c r="V10" t="s">
-        <v>66</v>
-      </c>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
+      <c r="Y10" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>70</v>
+      </c>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
+      <c r="AG10" t="s">
+        <v>51</v>
+      </c>
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
@@ -3167,7 +3317,9 @@
       <c r="I11" s="1">
         <v>3</v>
       </c>
-      <c r="J11" s="1"/>
+      <c r="J11" s="1">
+        <v>3</v>
+      </c>
       <c r="K11" t="s">
         <v>53</v>
       </c>
@@ -3181,40 +3333,50 @@
         <v>57</v>
       </c>
       <c r="O11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q11" t="s">
+        <v>67</v>
+      </c>
+      <c r="R11" t="s">
+        <v>70</v>
+      </c>
+      <c r="S11" t="s">
+        <v>61</v>
+      </c>
+      <c r="T11" t="s">
         <v>64</v>
       </c>
-      <c r="R11" t="s">
-        <v>66</v>
-      </c>
-      <c r="S11" t="s">
-        <v>60</v>
-      </c>
-      <c r="T11" t="s">
-        <v>62</v>
-      </c>
       <c r="U11" t="s">
+        <v>67</v>
+      </c>
+      <c r="V11" t="s">
+        <v>70</v>
+      </c>
+      <c r="W11" t="s">
+        <v>72</v>
+      </c>
+      <c r="X11" t="s">
         <v>64</v>
       </c>
-      <c r="V11" t="s">
-        <v>66</v>
-      </c>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
+      <c r="Y11" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>70</v>
+      </c>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
-      <c r="AG11" s="1"/>
+      <c r="AG11" t="s">
+        <v>51</v>
+      </c>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
@@ -3381,7 +3543,9 @@
       <c r="I12" s="1">
         <v>2</v>
       </c>
-      <c r="J12" s="1"/>
+      <c r="J12" s="1">
+        <v>2</v>
+      </c>
       <c r="K12" t="s">
         <v>53</v>
       </c>
@@ -3395,40 +3559,50 @@
         <v>57</v>
       </c>
       <c r="O12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q12" t="s">
+        <v>67</v>
+      </c>
+      <c r="R12" t="s">
+        <v>70</v>
+      </c>
+      <c r="S12" t="s">
+        <v>61</v>
+      </c>
+      <c r="T12" t="s">
         <v>64</v>
       </c>
-      <c r="R12" t="s">
-        <v>66</v>
-      </c>
-      <c r="S12" t="s">
-        <v>60</v>
-      </c>
-      <c r="T12" t="s">
-        <v>62</v>
-      </c>
       <c r="U12" t="s">
+        <v>67</v>
+      </c>
+      <c r="V12" t="s">
+        <v>70</v>
+      </c>
+      <c r="W12" t="s">
+        <v>72</v>
+      </c>
+      <c r="X12" t="s">
         <v>64</v>
       </c>
-      <c r="V12" t="s">
-        <v>66</v>
-      </c>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
+      <c r="Y12" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>70</v>
+      </c>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
-      <c r="AG12" s="1"/>
+      <c r="AG12" t="s">
+        <v>51</v>
+      </c>
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
@@ -3595,7 +3769,9 @@
       <c r="I13" s="1">
         <v>3</v>
       </c>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1">
+        <v>3</v>
+      </c>
       <c r="K13" t="s">
         <v>53</v>
       </c>
@@ -3609,40 +3785,50 @@
         <v>57</v>
       </c>
       <c r="O13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q13" t="s">
+        <v>67</v>
+      </c>
+      <c r="R13" t="s">
+        <v>70</v>
+      </c>
+      <c r="S13" t="s">
+        <v>61</v>
+      </c>
+      <c r="T13" t="s">
         <v>64</v>
       </c>
-      <c r="R13" t="s">
-        <v>66</v>
-      </c>
-      <c r="S13" t="s">
-        <v>60</v>
-      </c>
-      <c r="T13" t="s">
-        <v>62</v>
-      </c>
       <c r="U13" t="s">
+        <v>67</v>
+      </c>
+      <c r="V13" t="s">
+        <v>70</v>
+      </c>
+      <c r="W13" t="s">
+        <v>72</v>
+      </c>
+      <c r="X13" t="s">
         <v>64</v>
       </c>
-      <c r="V13" t="s">
-        <v>66</v>
-      </c>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
+      <c r="Y13" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>70</v>
+      </c>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
-      <c r="AG13" s="1"/>
+      <c r="AG13" t="s">
+        <v>51</v>
+      </c>
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
       <c r="AJ13" s="1"/>
@@ -3809,7 +3995,9 @@
       <c r="I14" s="1">
         <v>2</v>
       </c>
-      <c r="J14" s="1"/>
+      <c r="J14" s="1">
+        <v>2</v>
+      </c>
       <c r="K14" t="s">
         <v>53</v>
       </c>
@@ -3823,40 +4011,50 @@
         <v>57</v>
       </c>
       <c r="O14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q14" t="s">
+        <v>67</v>
+      </c>
+      <c r="R14" t="s">
+        <v>70</v>
+      </c>
+      <c r="S14" t="s">
+        <v>61</v>
+      </c>
+      <c r="T14" t="s">
         <v>64</v>
       </c>
-      <c r="R14" t="s">
-        <v>66</v>
-      </c>
-      <c r="S14" t="s">
-        <v>60</v>
-      </c>
-      <c r="T14" t="s">
-        <v>62</v>
-      </c>
       <c r="U14" t="s">
+        <v>67</v>
+      </c>
+      <c r="V14" t="s">
+        <v>70</v>
+      </c>
+      <c r="W14" t="s">
+        <v>72</v>
+      </c>
+      <c r="X14" t="s">
         <v>64</v>
       </c>
-      <c r="V14" t="s">
-        <v>66</v>
-      </c>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
+      <c r="Y14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>70</v>
+      </c>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
-      <c r="AG14" s="1"/>
+      <c r="AG14" t="s">
+        <v>51</v>
+      </c>
       <c r="AH14" s="1"/>
       <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
@@ -4023,7 +4221,9 @@
       <c r="I15" s="1">
         <v>4</v>
       </c>
-      <c r="J15" s="1"/>
+      <c r="J15" s="1">
+        <v>3</v>
+      </c>
       <c r="K15" t="s">
         <v>53</v>
       </c>
@@ -4037,40 +4237,50 @@
         <v>57</v>
       </c>
       <c r="O15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q15" t="s">
+        <v>67</v>
+      </c>
+      <c r="R15" t="s">
+        <v>70</v>
+      </c>
+      <c r="S15" t="s">
+        <v>61</v>
+      </c>
+      <c r="T15" t="s">
         <v>64</v>
       </c>
-      <c r="R15" t="s">
-        <v>66</v>
-      </c>
-      <c r="S15" t="s">
-        <v>60</v>
-      </c>
-      <c r="T15" t="s">
-        <v>62</v>
-      </c>
       <c r="U15" t="s">
+        <v>67</v>
+      </c>
+      <c r="V15" t="s">
+        <v>70</v>
+      </c>
+      <c r="W15" t="s">
+        <v>72</v>
+      </c>
+      <c r="X15" t="s">
         <v>64</v>
       </c>
-      <c r="V15" t="s">
-        <v>66</v>
-      </c>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
+      <c r="Y15" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>70</v>
+      </c>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
-      <c r="AG15" s="1"/>
+      <c r="AG15" t="s">
+        <v>51</v>
+      </c>
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
@@ -4235,9 +4445,11 @@
         <v>12</v>
       </c>
       <c r="I16" s="1">
-        <v>2</v>
-      </c>
-      <c r="J16" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="J16" s="1">
+        <v>3</v>
+      </c>
       <c r="K16" t="s">
         <v>53</v>
       </c>
@@ -4251,40 +4463,50 @@
         <v>57</v>
       </c>
       <c r="O16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q16" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" t="s">
+        <v>70</v>
+      </c>
+      <c r="S16" t="s">
+        <v>61</v>
+      </c>
+      <c r="T16" t="s">
         <v>64</v>
       </c>
-      <c r="R16" t="s">
-        <v>66</v>
-      </c>
-      <c r="S16" t="s">
-        <v>60</v>
-      </c>
-      <c r="T16" t="s">
-        <v>62</v>
-      </c>
       <c r="U16" t="s">
+        <v>67</v>
+      </c>
+      <c r="V16" t="s">
+        <v>70</v>
+      </c>
+      <c r="W16" t="s">
+        <v>72</v>
+      </c>
+      <c r="X16" t="s">
         <v>64</v>
       </c>
-      <c r="V16" t="s">
-        <v>66</v>
-      </c>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
+      <c r="Y16" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>70</v>
+      </c>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
-      <c r="AG16" s="1"/>
+      <c r="AG16" t="s">
+        <v>51</v>
+      </c>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
@@ -4451,7 +4673,9 @@
       <c r="I17" s="1">
         <v>2</v>
       </c>
-      <c r="J17" s="1"/>
+      <c r="J17" s="1">
+        <v>2</v>
+      </c>
       <c r="K17" t="s">
         <v>53</v>
       </c>
@@ -4465,40 +4689,50 @@
         <v>57</v>
       </c>
       <c r="O17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q17" t="s">
+        <v>67</v>
+      </c>
+      <c r="R17" t="s">
+        <v>70</v>
+      </c>
+      <c r="S17" t="s">
+        <v>61</v>
+      </c>
+      <c r="T17" t="s">
         <v>64</v>
       </c>
-      <c r="R17" t="s">
-        <v>66</v>
-      </c>
-      <c r="S17" t="s">
-        <v>60</v>
-      </c>
-      <c r="T17" t="s">
-        <v>62</v>
-      </c>
       <c r="U17" t="s">
+        <v>67</v>
+      </c>
+      <c r="V17" t="s">
+        <v>70</v>
+      </c>
+      <c r="W17" t="s">
+        <v>72</v>
+      </c>
+      <c r="X17" t="s">
         <v>64</v>
       </c>
-      <c r="V17" t="s">
-        <v>66</v>
-      </c>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
+      <c r="Y17" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>70</v>
+      </c>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
-      <c r="AG17" s="1"/>
+      <c r="AG17" t="s">
+        <v>51</v>
+      </c>
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
@@ -4665,7 +4899,9 @@
       <c r="I18" s="1">
         <v>1</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
       <c r="K18" t="s">
         <v>53</v>
       </c>
@@ -4679,40 +4915,50 @@
         <v>57</v>
       </c>
       <c r="O18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q18" t="s">
+        <v>67</v>
+      </c>
+      <c r="R18" t="s">
+        <v>70</v>
+      </c>
+      <c r="S18" t="s">
+        <v>61</v>
+      </c>
+      <c r="T18" t="s">
         <v>64</v>
       </c>
-      <c r="R18" t="s">
-        <v>66</v>
-      </c>
-      <c r="S18" t="s">
-        <v>60</v>
-      </c>
-      <c r="T18" t="s">
-        <v>62</v>
-      </c>
       <c r="U18" t="s">
+        <v>67</v>
+      </c>
+      <c r="V18" t="s">
+        <v>70</v>
+      </c>
+      <c r="W18" t="s">
+        <v>72</v>
+      </c>
+      <c r="X18" t="s">
         <v>64</v>
       </c>
-      <c r="V18" t="s">
-        <v>66</v>
-      </c>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
+      <c r="Y18" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>70</v>
+      </c>
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
-      <c r="AG18" s="1"/>
+      <c r="AG18" t="s">
+        <v>51</v>
+      </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
@@ -4879,7 +5125,9 @@
       <c r="I19" s="1">
         <v>2</v>
       </c>
-      <c r="J19" s="1"/>
+      <c r="J19" s="1">
+        <v>2</v>
+      </c>
       <c r="K19" t="s">
         <v>53</v>
       </c>
@@ -4893,40 +5141,50 @@
         <v>57</v>
       </c>
       <c r="O19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q19" t="s">
+        <v>67</v>
+      </c>
+      <c r="R19" t="s">
+        <v>70</v>
+      </c>
+      <c r="S19" t="s">
+        <v>61</v>
+      </c>
+      <c r="T19" t="s">
         <v>64</v>
       </c>
-      <c r="R19" t="s">
-        <v>66</v>
-      </c>
-      <c r="S19" t="s">
-        <v>60</v>
-      </c>
-      <c r="T19" t="s">
-        <v>62</v>
-      </c>
       <c r="U19" t="s">
+        <v>67</v>
+      </c>
+      <c r="V19" t="s">
+        <v>70</v>
+      </c>
+      <c r="W19" t="s">
+        <v>72</v>
+      </c>
+      <c r="X19" t="s">
         <v>64</v>
       </c>
-      <c r="V19" t="s">
-        <v>66</v>
-      </c>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
+      <c r="Y19" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>70</v>
+      </c>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
-      <c r="AG19" s="1"/>
+      <c r="AG19" t="s">
+        <v>51</v>
+      </c>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
       <c r="AJ19" s="1"/>
@@ -5093,7 +5351,9 @@
       <c r="I20" s="1">
         <v>3</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="1">
+        <v>3</v>
+      </c>
       <c r="K20" t="s">
         <v>53</v>
       </c>
@@ -5107,40 +5367,50 @@
         <v>57</v>
       </c>
       <c r="O20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q20" t="s">
+        <v>67</v>
+      </c>
+      <c r="R20" t="s">
+        <v>70</v>
+      </c>
+      <c r="S20" t="s">
+        <v>61</v>
+      </c>
+      <c r="T20" t="s">
         <v>64</v>
       </c>
-      <c r="R20" t="s">
-        <v>66</v>
-      </c>
-      <c r="S20" t="s">
-        <v>60</v>
-      </c>
-      <c r="T20" t="s">
-        <v>62</v>
-      </c>
       <c r="U20" t="s">
+        <v>67</v>
+      </c>
+      <c r="V20" t="s">
+        <v>70</v>
+      </c>
+      <c r="W20" t="s">
+        <v>72</v>
+      </c>
+      <c r="X20" t="s">
         <v>64</v>
       </c>
-      <c r="V20" t="s">
-        <v>66</v>
-      </c>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
+      <c r="Y20" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>70</v>
+      </c>
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
       <c r="AE20" s="1"/>
       <c r="AF20" s="1"/>
-      <c r="AG20" s="1"/>
+      <c r="AG20" t="s">
+        <v>51</v>
+      </c>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
       <c r="AJ20" s="1"/>
@@ -5307,7 +5577,9 @@
       <c r="I21" s="1">
         <v>3</v>
       </c>
-      <c r="J21" s="1"/>
+      <c r="J21" s="1">
+        <v>2</v>
+      </c>
       <c r="K21" t="s">
         <v>53</v>
       </c>
@@ -5321,40 +5593,50 @@
         <v>57</v>
       </c>
       <c r="O21" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q21" t="s">
+        <v>67</v>
+      </c>
+      <c r="R21" t="s">
+        <v>70</v>
+      </c>
+      <c r="S21" t="s">
+        <v>72</v>
+      </c>
+      <c r="T21" t="s">
         <v>64</v>
       </c>
-      <c r="R21" t="s">
-        <v>66</v>
-      </c>
-      <c r="S21" t="s">
-        <v>51</v>
-      </c>
-      <c r="T21" t="s">
-        <v>51</v>
-      </c>
       <c r="U21" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="V21" t="s">
-        <v>51</v>
-      </c>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W21" t="s">
+        <v>51</v>
+      </c>
+      <c r="X21" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>51</v>
+      </c>
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
-      <c r="AG21" s="1"/>
+      <c r="AG21" t="s">
+        <v>51</v>
+      </c>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
@@ -5521,7 +5803,9 @@
       <c r="I22" s="1">
         <v>3</v>
       </c>
-      <c r="J22" s="1"/>
+      <c r="J22" s="1">
+        <v>2</v>
+      </c>
       <c r="K22" t="s">
         <v>53</v>
       </c>
@@ -5535,40 +5819,50 @@
         <v>57</v>
       </c>
       <c r="O22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P22" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q22" t="s">
+        <v>67</v>
+      </c>
+      <c r="R22" t="s">
+        <v>70</v>
+      </c>
+      <c r="S22" t="s">
+        <v>72</v>
+      </c>
+      <c r="T22" t="s">
         <v>64</v>
       </c>
-      <c r="R22" t="s">
-        <v>66</v>
-      </c>
-      <c r="S22" t="s">
-        <v>51</v>
-      </c>
-      <c r="T22" t="s">
-        <v>51</v>
-      </c>
       <c r="U22" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="V22" t="s">
-        <v>51</v>
-      </c>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W22" t="s">
+        <v>51</v>
+      </c>
+      <c r="X22" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>51</v>
+      </c>
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
       <c r="AE22" s="1"/>
       <c r="AF22" s="1"/>
-      <c r="AG22" s="1"/>
+      <c r="AG22" t="s">
+        <v>51</v>
+      </c>
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
@@ -5735,7 +6029,9 @@
       <c r="I23" s="1">
         <v>3</v>
       </c>
-      <c r="J23" s="1"/>
+      <c r="J23" s="1">
+        <v>2</v>
+      </c>
       <c r="K23" t="s">
         <v>53</v>
       </c>
@@ -5749,40 +6045,50 @@
         <v>57</v>
       </c>
       <c r="O23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q23" t="s">
+        <v>67</v>
+      </c>
+      <c r="R23" t="s">
+        <v>70</v>
+      </c>
+      <c r="S23" t="s">
+        <v>72</v>
+      </c>
+      <c r="T23" t="s">
         <v>64</v>
       </c>
-      <c r="R23" t="s">
-        <v>66</v>
-      </c>
-      <c r="S23" t="s">
-        <v>51</v>
-      </c>
-      <c r="T23" t="s">
-        <v>51</v>
-      </c>
       <c r="U23" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="V23" t="s">
-        <v>51</v>
-      </c>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W23" t="s">
+        <v>51</v>
+      </c>
+      <c r="X23" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>51</v>
+      </c>
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
       <c r="AE23" s="1"/>
       <c r="AF23" s="1"/>
-      <c r="AG23" s="1"/>
+      <c r="AG23" t="s">
+        <v>51</v>
+      </c>
       <c r="AH23" s="1"/>
       <c r="AI23" s="1"/>
       <c r="AJ23" s="1"/>
@@ -5949,7 +6255,9 @@
       <c r="I24" s="1">
         <v>3</v>
       </c>
-      <c r="J24" s="1"/>
+      <c r="J24" s="1">
+        <v>2</v>
+      </c>
       <c r="K24" t="s">
         <v>53</v>
       </c>
@@ -5963,40 +6271,50 @@
         <v>57</v>
       </c>
       <c r="O24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q24" t="s">
+        <v>67</v>
+      </c>
+      <c r="R24" t="s">
+        <v>70</v>
+      </c>
+      <c r="S24" t="s">
+        <v>72</v>
+      </c>
+      <c r="T24" t="s">
         <v>64</v>
       </c>
-      <c r="R24" t="s">
-        <v>66</v>
-      </c>
-      <c r="S24" t="s">
-        <v>51</v>
-      </c>
-      <c r="T24" t="s">
-        <v>51</v>
-      </c>
       <c r="U24" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="V24" t="s">
-        <v>51</v>
-      </c>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W24" t="s">
+        <v>51</v>
+      </c>
+      <c r="X24" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>51</v>
+      </c>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
       <c r="AE24" s="1"/>
       <c r="AF24" s="1"/>
-      <c r="AG24" s="1"/>
+      <c r="AG24" t="s">
+        <v>51</v>
+      </c>
       <c r="AH24" s="1"/>
       <c r="AI24" s="1"/>
       <c r="AJ24" s="1"/>
@@ -6163,7 +6481,9 @@
       <c r="I25" s="1">
         <v>3</v>
       </c>
-      <c r="J25" s="1"/>
+      <c r="J25" s="1">
+        <v>2</v>
+      </c>
       <c r="K25" t="s">
         <v>53</v>
       </c>
@@ -6177,40 +6497,50 @@
         <v>57</v>
       </c>
       <c r="O25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P25" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q25" t="s">
+        <v>67</v>
+      </c>
+      <c r="R25" t="s">
+        <v>70</v>
+      </c>
+      <c r="S25" t="s">
+        <v>72</v>
+      </c>
+      <c r="T25" t="s">
         <v>64</v>
       </c>
-      <c r="R25" t="s">
-        <v>66</v>
-      </c>
-      <c r="S25" t="s">
-        <v>51</v>
-      </c>
-      <c r="T25" t="s">
-        <v>51</v>
-      </c>
       <c r="U25" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="V25" t="s">
-        <v>51</v>
-      </c>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W25" t="s">
+        <v>51</v>
+      </c>
+      <c r="X25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>51</v>
+      </c>
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
       <c r="AF25" s="1"/>
-      <c r="AG25" s="1"/>
+      <c r="AG25" t="s">
+        <v>51</v>
+      </c>
       <c r="AH25" s="1"/>
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
@@ -6377,7 +6707,9 @@
       <c r="I26" s="1">
         <v>2</v>
       </c>
-      <c r="J26" s="1"/>
+      <c r="J26" s="1">
+        <v>2</v>
+      </c>
       <c r="K26" t="s">
         <v>53</v>
       </c>
@@ -6391,40 +6723,50 @@
         <v>57</v>
       </c>
       <c r="O26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P26" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q26" t="s">
+        <v>67</v>
+      </c>
+      <c r="R26" t="s">
+        <v>70</v>
+      </c>
+      <c r="S26" t="s">
+        <v>72</v>
+      </c>
+      <c r="T26" t="s">
         <v>64</v>
       </c>
-      <c r="R26" t="s">
-        <v>66</v>
-      </c>
-      <c r="S26" t="s">
-        <v>51</v>
-      </c>
-      <c r="T26" t="s">
-        <v>51</v>
-      </c>
       <c r="U26" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="V26" t="s">
-        <v>51</v>
-      </c>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-      <c r="Z26" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W26" t="s">
+        <v>51</v>
+      </c>
+      <c r="X26" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>51</v>
+      </c>
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
       <c r="AF26" s="1"/>
-      <c r="AG26" s="1"/>
+      <c r="AG26" t="s">
+        <v>51</v>
+      </c>
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
       <c r="AJ26" s="1"/>
@@ -6585,9 +6927,15 @@
       <c r="G27" s="1">
         <v>3</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="H27" s="1">
+        <v>12</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
       <c r="K27" t="s">
         <v>53</v>
       </c>
@@ -6601,40 +6949,50 @@
         <v>57</v>
       </c>
       <c r="O27" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q27" t="s">
+        <v>67</v>
+      </c>
+      <c r="R27" t="s">
+        <v>70</v>
+      </c>
+      <c r="S27" t="s">
+        <v>72</v>
+      </c>
+      <c r="T27" t="s">
         <v>64</v>
       </c>
-      <c r="R27" t="s">
-        <v>66</v>
-      </c>
-      <c r="S27" t="s">
-        <v>51</v>
-      </c>
-      <c r="T27" t="s">
-        <v>51</v>
-      </c>
       <c r="U27" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="V27" t="s">
-        <v>51</v>
-      </c>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W27" t="s">
+        <v>51</v>
+      </c>
+      <c r="X27" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>51</v>
+      </c>
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
       <c r="AE27" s="1"/>
       <c r="AF27" s="1"/>
-      <c r="AG27" s="1"/>
+      <c r="AG27" t="s">
+        <v>51</v>
+      </c>
       <c r="AH27" s="1"/>
       <c r="AI27" s="1"/>
       <c r="AJ27" s="1"/>
@@ -6801,7 +7159,9 @@
       <c r="I28" s="1">
         <v>3</v>
       </c>
-      <c r="J28" s="1"/>
+      <c r="J28" s="1">
+        <v>3</v>
+      </c>
       <c r="K28" t="s">
         <v>53</v>
       </c>
@@ -6815,40 +7175,50 @@
         <v>57</v>
       </c>
       <c r="O28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P28" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q28" t="s">
+        <v>67</v>
+      </c>
+      <c r="R28" t="s">
+        <v>70</v>
+      </c>
+      <c r="S28" t="s">
+        <v>72</v>
+      </c>
+      <c r="T28" t="s">
         <v>64</v>
       </c>
-      <c r="R28" t="s">
-        <v>66</v>
-      </c>
-      <c r="S28" t="s">
-        <v>51</v>
-      </c>
-      <c r="T28" t="s">
-        <v>51</v>
-      </c>
       <c r="U28" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="V28" t="s">
-        <v>51</v>
-      </c>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W28" t="s">
+        <v>51</v>
+      </c>
+      <c r="X28" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>51</v>
+      </c>
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
       <c r="AE28" s="1"/>
       <c r="AF28" s="1"/>
-      <c r="AG28" s="1"/>
+      <c r="AG28" t="s">
+        <v>51</v>
+      </c>
       <c r="AH28" s="1"/>
       <c r="AI28" s="1"/>
       <c r="AJ28" s="1"/>
@@ -7015,7 +7385,9 @@
       <c r="I29" s="1">
         <v>4</v>
       </c>
-      <c r="J29" s="1"/>
+      <c r="J29" s="1">
+        <v>3</v>
+      </c>
       <c r="K29" t="s">
         <v>53</v>
       </c>
@@ -7029,40 +7401,50 @@
         <v>57</v>
       </c>
       <c r="O29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P29" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q29" t="s">
+        <v>67</v>
+      </c>
+      <c r="R29" t="s">
+        <v>70</v>
+      </c>
+      <c r="S29" t="s">
+        <v>72</v>
+      </c>
+      <c r="T29" t="s">
         <v>64</v>
       </c>
-      <c r="R29" t="s">
-        <v>66</v>
-      </c>
-      <c r="S29" t="s">
-        <v>51</v>
-      </c>
-      <c r="T29" t="s">
-        <v>51</v>
-      </c>
       <c r="U29" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="V29" t="s">
-        <v>51</v>
-      </c>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W29" t="s">
+        <v>51</v>
+      </c>
+      <c r="X29" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>51</v>
+      </c>
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
       <c r="AE29" s="1"/>
       <c r="AF29" s="1"/>
-      <c r="AG29" s="1"/>
+      <c r="AG29" t="s">
+        <v>51</v>
+      </c>
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
       <c r="AJ29" s="1"/>
@@ -7229,7 +7611,9 @@
       <c r="I30" s="1">
         <v>1</v>
       </c>
-      <c r="J30" s="1"/>
+      <c r="J30" s="1">
+        <v>1</v>
+      </c>
       <c r="K30" t="s">
         <v>53</v>
       </c>
@@ -7243,40 +7627,50 @@
         <v>57</v>
       </c>
       <c r="O30" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P30" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q30" t="s">
+        <v>67</v>
+      </c>
+      <c r="R30" t="s">
+        <v>70</v>
+      </c>
+      <c r="S30" t="s">
+        <v>72</v>
+      </c>
+      <c r="T30" t="s">
         <v>64</v>
       </c>
-      <c r="R30" t="s">
-        <v>66</v>
-      </c>
-      <c r="S30" t="s">
-        <v>51</v>
-      </c>
-      <c r="T30" t="s">
-        <v>51</v>
-      </c>
       <c r="U30" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="V30" t="s">
-        <v>51</v>
-      </c>
-      <c r="W30" s="1"/>
-      <c r="X30" s="1"/>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W30" t="s">
+        <v>51</v>
+      </c>
+      <c r="X30" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>51</v>
+      </c>
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
       <c r="AE30" s="1"/>
       <c r="AF30" s="1"/>
-      <c r="AG30" s="1"/>
+      <c r="AG30" t="s">
+        <v>51</v>
+      </c>
       <c r="AH30" s="1"/>
       <c r="AI30" s="1"/>
       <c r="AJ30" s="1"/>
@@ -7443,7 +7837,9 @@
       <c r="I31" s="1">
         <v>3</v>
       </c>
-      <c r="J31" s="1"/>
+      <c r="J31" s="1">
+        <v>3</v>
+      </c>
       <c r="K31" t="s">
         <v>53</v>
       </c>
@@ -7457,40 +7853,50 @@
         <v>57</v>
       </c>
       <c r="O31" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P31" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q31" t="s">
+        <v>67</v>
+      </c>
+      <c r="R31" t="s">
+        <v>70</v>
+      </c>
+      <c r="S31" t="s">
+        <v>72</v>
+      </c>
+      <c r="T31" t="s">
         <v>64</v>
       </c>
-      <c r="R31" t="s">
-        <v>66</v>
-      </c>
-      <c r="S31" t="s">
-        <v>51</v>
-      </c>
-      <c r="T31" t="s">
-        <v>51</v>
-      </c>
       <c r="U31" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="V31" t="s">
-        <v>51</v>
-      </c>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W31" t="s">
+        <v>51</v>
+      </c>
+      <c r="X31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>51</v>
+      </c>
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
       <c r="AE31" s="1"/>
       <c r="AF31" s="1"/>
-      <c r="AG31" s="1"/>
+      <c r="AG31" t="s">
+        <v>51</v>
+      </c>
       <c r="AH31" s="1"/>
       <c r="AI31" s="1"/>
       <c r="AJ31" s="1"/>
@@ -7657,7 +8063,9 @@
       <c r="I32" s="1">
         <v>3</v>
       </c>
-      <c r="J32" s="1"/>
+      <c r="J32" s="1">
+        <v>3</v>
+      </c>
       <c r="K32" t="s">
         <v>53</v>
       </c>
@@ -7671,40 +8079,50 @@
         <v>57</v>
       </c>
       <c r="O32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P32" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q32" t="s">
+        <v>67</v>
+      </c>
+      <c r="R32" t="s">
+        <v>70</v>
+      </c>
+      <c r="S32" t="s">
+        <v>72</v>
+      </c>
+      <c r="T32" t="s">
         <v>64</v>
       </c>
-      <c r="R32" t="s">
-        <v>66</v>
-      </c>
-      <c r="S32" t="s">
-        <v>51</v>
-      </c>
-      <c r="T32" t="s">
-        <v>51</v>
-      </c>
       <c r="U32" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="V32" t="s">
-        <v>51</v>
-      </c>
-      <c r="W32" s="1"/>
-      <c r="X32" s="1"/>
-      <c r="Y32" s="1"/>
-      <c r="Z32" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W32" t="s">
+        <v>51</v>
+      </c>
+      <c r="X32" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>51</v>
+      </c>
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
       <c r="AE32" s="1"/>
       <c r="AF32" s="1"/>
-      <c r="AG32" s="1"/>
+      <c r="AG32" t="s">
+        <v>51</v>
+      </c>
       <c r="AH32" s="1"/>
       <c r="AI32" s="1"/>
       <c r="AJ32" s="1"/>
@@ -7871,7 +8289,9 @@
       <c r="I33" s="1">
         <v>3</v>
       </c>
-      <c r="J33" s="1"/>
+      <c r="J33" s="1">
+        <v>3</v>
+      </c>
       <c r="K33" t="s">
         <v>53</v>
       </c>
@@ -7885,40 +8305,50 @@
         <v>57</v>
       </c>
       <c r="O33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P33" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q33" t="s">
+        <v>67</v>
+      </c>
+      <c r="R33" t="s">
+        <v>70</v>
+      </c>
+      <c r="S33" t="s">
+        <v>72</v>
+      </c>
+      <c r="T33" t="s">
         <v>64</v>
       </c>
-      <c r="R33" t="s">
-        <v>66</v>
-      </c>
-      <c r="S33" t="s">
-        <v>51</v>
-      </c>
-      <c r="T33" t="s">
-        <v>51</v>
-      </c>
       <c r="U33" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="V33" t="s">
-        <v>51</v>
-      </c>
-      <c r="W33" s="1"/>
-      <c r="X33" s="1"/>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="W33" t="s">
+        <v>51</v>
+      </c>
+      <c r="X33" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>51</v>
+      </c>
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
       <c r="AE33" s="1"/>
       <c r="AF33" s="1"/>
-      <c r="AG33" s="1"/>
+      <c r="AG33" t="s">
+        <v>51</v>
+      </c>
       <c r="AH33" s="1"/>
       <c r="AI33" s="1"/>
       <c r="AJ33" s="1"/>

</xml_diff>

<commit_message>
update to 2024 data
</commit_message>
<xml_diff>
--- a/analytics/modified_data/tbf_market_garden_data_2024_clean.xlsx
+++ b/analytics/modified_data/tbf_market_garden_data_2024_clean.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="778" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="906" uniqueCount="226">
   <si>
     <t>crop</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>sow_fert_date_3</t>
+  </si>
+  <si>
+    <t>2024-04-23</t>
   </si>
   <si>
     <t>sow_fert_type_npk_3</t>
@@ -810,445 +813,445 @@
         <v>76</v>
       </c>
       <c r="X1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="Y1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Z1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AA1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AB1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AC1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AD1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AE1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AF1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AG1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AI1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AJ1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AK1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AL1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AM1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AN1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AO1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AP1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AQ1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AR1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AS1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AT1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AU1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AV1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AW1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AX1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AY1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AZ1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="BA1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="BB1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="BC1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="BD1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="BE1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="BF1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="BG1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="BH1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="BI1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="BJ1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="BK1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="BL1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="BM1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="BN1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="BO1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="BP1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="BQ1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="BR1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BT1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="BU1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="BV1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="BW1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="BX1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BY1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BZ1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="CA1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="CB1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="CC1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="CD1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="CE1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="CF1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CG1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CH1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CI1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CJ1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="CK1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CL1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CM1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CN1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CO1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CP1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="CQ1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="CR1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="CS1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="CT1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="CU1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="CV1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="CW1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="CX1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="CY1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="CZ1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="DA1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="DB1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="DC1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="DD1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="DE1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="DF1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="DG1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="DH1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="DI1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="DJ1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="DK1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="DL1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="DM1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="DN1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="DO1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="DP1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="DQ1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="DR1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="DS1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="DT1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="DU1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="DV1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="DW1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="DX1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DY1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="DZ1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="EA1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="EB1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="EC1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="ED1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="EE1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="EF1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="EG1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="EH1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="EI1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="EJ1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="EK1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="EL1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="EM1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="EN1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="EO1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="EP1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="EQ1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="ER1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="ES1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="ET1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="EU1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="EV1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="EW1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="EX1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="EY1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="EZ1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="FA1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="FB1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="FC1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="FD1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="FE1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="FF1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="FG1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="FH1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="FI1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="FJ1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="FK1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="FL1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="FM1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="FN1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2">
@@ -1322,10 +1325,18 @@
       <c r="Z2" t="s">
         <v>51</v>
       </c>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
+      <c r="AA2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>51</v>
+      </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
       <c r="AG2" t="s">
@@ -1546,14 +1557,22 @@
       <c r="Z3" t="s">
         <v>51</v>
       </c>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
+      <c r="AA3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>51</v>
+      </c>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
       <c r="AG3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AH3" s="1">
         <v>3.25</v>
@@ -1774,14 +1793,22 @@
       <c r="Z4" t="s">
         <v>51</v>
       </c>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
+      <c r="AA4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>51</v>
+      </c>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
       <c r="AG4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AH4" s="1">
         <v>3.25</v>
@@ -2002,14 +2029,22 @@
       <c r="Z5" t="s">
         <v>51</v>
       </c>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
+      <c r="AA5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>51</v>
+      </c>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
       <c r="AG5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AH5" s="1">
         <v>3.25</v>
@@ -2230,14 +2265,22 @@
       <c r="Z6" t="s">
         <v>51</v>
       </c>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
+      <c r="AA6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>51</v>
+      </c>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
       <c r="AG6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AH6" s="1">
         <v>3.25</v>
@@ -2458,14 +2501,22 @@
       <c r="Z7" t="s">
         <v>51</v>
       </c>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
+      <c r="AA7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>51</v>
+      </c>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
       <c r="AG7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AH7" s="1">
         <v>3.25</v>
@@ -2686,14 +2737,22 @@
       <c r="Z8" t="s">
         <v>51</v>
       </c>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
+      <c r="AA8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>51</v>
+      </c>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
       <c r="AG8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AH8" s="1">
         <v>3.25</v>
@@ -2916,10 +2975,18 @@
       <c r="Z9" t="s">
         <v>70</v>
       </c>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
+      <c r="AA9" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>70</v>
+      </c>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
       <c r="AG9" t="s">
@@ -3142,10 +3209,18 @@
       <c r="Z10" t="s">
         <v>70</v>
       </c>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
+      <c r="AA10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>70</v>
+      </c>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
       <c r="AG10" t="s">
@@ -3368,10 +3443,18 @@
       <c r="Z11" t="s">
         <v>70</v>
       </c>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
+      <c r="AA11" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>70</v>
+      </c>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
       <c r="AG11" t="s">
@@ -3594,10 +3677,18 @@
       <c r="Z12" t="s">
         <v>70</v>
       </c>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
+      <c r="AA12" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>70</v>
+      </c>
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
       <c r="AG12" t="s">
@@ -3820,10 +3911,18 @@
       <c r="Z13" t="s">
         <v>70</v>
       </c>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
-      <c r="AD13" s="1"/>
+      <c r="AA13" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>70</v>
+      </c>
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
       <c r="AG13" t="s">
@@ -4046,10 +4145,18 @@
       <c r="Z14" t="s">
         <v>70</v>
       </c>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
+      <c r="AA14" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>70</v>
+      </c>
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
       <c r="AG14" t="s">
@@ -4272,10 +4379,18 @@
       <c r="Z15" t="s">
         <v>70</v>
       </c>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1"/>
-      <c r="AD15" s="1"/>
+      <c r="AA15" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>70</v>
+      </c>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
       <c r="AG15" t="s">
@@ -4498,10 +4613,18 @@
       <c r="Z16" t="s">
         <v>70</v>
       </c>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
+      <c r="AA16" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>70</v>
+      </c>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
       <c r="AG16" t="s">
@@ -4724,10 +4847,18 @@
       <c r="Z17" t="s">
         <v>70</v>
       </c>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
-      <c r="AD17" s="1"/>
+      <c r="AA17" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>70</v>
+      </c>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
       <c r="AG17" t="s">
@@ -4950,10 +5081,18 @@
       <c r="Z18" t="s">
         <v>70</v>
       </c>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
-      <c r="AD18" s="1"/>
+      <c r="AA18" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>70</v>
+      </c>
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
       <c r="AG18" t="s">
@@ -5176,10 +5315,18 @@
       <c r="Z19" t="s">
         <v>70</v>
       </c>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
+      <c r="AA19" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>70</v>
+      </c>
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
       <c r="AG19" t="s">
@@ -5402,10 +5549,18 @@
       <c r="Z20" t="s">
         <v>70</v>
       </c>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-      <c r="AD20" s="1"/>
+      <c r="AA20" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>70</v>
+      </c>
       <c r="AE20" s="1"/>
       <c r="AF20" s="1"/>
       <c r="AG20" t="s">
@@ -5617,21 +5772,29 @@
         <v>70</v>
       </c>
       <c r="W21" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="X21" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="Y21" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="Z21" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-      <c r="AD21" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>51</v>
+      </c>
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
       <c r="AG21" t="s">
@@ -5843,21 +6006,29 @@
         <v>70</v>
       </c>
       <c r="W22" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="X22" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="Y22" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="Z22" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA22" s="1"/>
-      <c r="AB22" s="1"/>
-      <c r="AC22" s="1"/>
-      <c r="AD22" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>51</v>
+      </c>
       <c r="AE22" s="1"/>
       <c r="AF22" s="1"/>
       <c r="AG22" t="s">
@@ -6069,21 +6240,29 @@
         <v>70</v>
       </c>
       <c r="W23" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="X23" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="Y23" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="Z23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA23" s="1"/>
-      <c r="AB23" s="1"/>
-      <c r="AC23" s="1"/>
-      <c r="AD23" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>51</v>
+      </c>
       <c r="AE23" s="1"/>
       <c r="AF23" s="1"/>
       <c r="AG23" t="s">
@@ -6295,21 +6474,29 @@
         <v>70</v>
       </c>
       <c r="W24" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="X24" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="Y24" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="Z24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA24" s="1"/>
-      <c r="AB24" s="1"/>
-      <c r="AC24" s="1"/>
-      <c r="AD24" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>51</v>
+      </c>
       <c r="AE24" s="1"/>
       <c r="AF24" s="1"/>
       <c r="AG24" t="s">
@@ -6521,21 +6708,29 @@
         <v>70</v>
       </c>
       <c r="W25" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="X25" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="Y25" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="Z25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA25" s="1"/>
-      <c r="AB25" s="1"/>
-      <c r="AC25" s="1"/>
-      <c r="AD25" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>51</v>
+      </c>
       <c r="AE25" s="1"/>
       <c r="AF25" s="1"/>
       <c r="AG25" t="s">
@@ -6747,21 +6942,29 @@
         <v>70</v>
       </c>
       <c r="W26" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="X26" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="Y26" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="Z26" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA26" s="1"/>
-      <c r="AB26" s="1"/>
-      <c r="AC26" s="1"/>
-      <c r="AD26" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>51</v>
+      </c>
       <c r="AE26" s="1"/>
       <c r="AF26" s="1"/>
       <c r="AG26" t="s">
@@ -6973,21 +7176,29 @@
         <v>70</v>
       </c>
       <c r="W27" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="X27" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="Y27" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="Z27" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA27" s="1"/>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
-      <c r="AD27" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>51</v>
+      </c>
       <c r="AE27" s="1"/>
       <c r="AF27" s="1"/>
       <c r="AG27" t="s">
@@ -7199,21 +7410,29 @@
         <v>70</v>
       </c>
       <c r="W28" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="X28" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="Y28" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="Z28" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA28" s="1"/>
-      <c r="AB28" s="1"/>
-      <c r="AC28" s="1"/>
-      <c r="AD28" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>51</v>
+      </c>
       <c r="AE28" s="1"/>
       <c r="AF28" s="1"/>
       <c r="AG28" t="s">
@@ -7425,21 +7644,29 @@
         <v>70</v>
       </c>
       <c r="W29" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="X29" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="Y29" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="Z29" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA29" s="1"/>
-      <c r="AB29" s="1"/>
-      <c r="AC29" s="1"/>
-      <c r="AD29" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>51</v>
+      </c>
       <c r="AE29" s="1"/>
       <c r="AF29" s="1"/>
       <c r="AG29" t="s">
@@ -7651,21 +7878,29 @@
         <v>70</v>
       </c>
       <c r="W30" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="X30" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="Y30" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="Z30" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA30" s="1"/>
-      <c r="AB30" s="1"/>
-      <c r="AC30" s="1"/>
-      <c r="AD30" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>51</v>
+      </c>
       <c r="AE30" s="1"/>
       <c r="AF30" s="1"/>
       <c r="AG30" t="s">
@@ -7877,21 +8112,29 @@
         <v>70</v>
       </c>
       <c r="W31" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="X31" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="Y31" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="Z31" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA31" s="1"/>
-      <c r="AB31" s="1"/>
-      <c r="AC31" s="1"/>
-      <c r="AD31" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>51</v>
+      </c>
       <c r="AE31" s="1"/>
       <c r="AF31" s="1"/>
       <c r="AG31" t="s">
@@ -8103,21 +8346,29 @@
         <v>70</v>
       </c>
       <c r="W32" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="X32" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="Y32" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="Z32" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA32" s="1"/>
-      <c r="AB32" s="1"/>
-      <c r="AC32" s="1"/>
-      <c r="AD32" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>51</v>
+      </c>
       <c r="AE32" s="1"/>
       <c r="AF32" s="1"/>
       <c r="AG32" t="s">
@@ -8329,21 +8580,29 @@
         <v>70</v>
       </c>
       <c r="W33" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="X33" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="Y33" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="Z33" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA33" s="1"/>
-      <c r="AB33" s="1"/>
-      <c r="AC33" s="1"/>
-      <c r="AD33" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>51</v>
+      </c>
       <c r="AE33" s="1"/>
       <c r="AF33" s="1"/>
       <c r="AG33" t="s">

</xml_diff>

<commit_message>
updates to 2024 harvest data
</commit_message>
<xml_diff>
--- a/analytics/modified_data/tbf_market_garden_data_2024_clean.xlsx
+++ b/analytics/modified_data/tbf_market_garden_data_2024_clean.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="7805" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="7953" uniqueCount="385">
   <si>
     <t>crop</t>
   </si>
@@ -949,6 +949,9 @@
   </si>
   <si>
     <t>harvest_date_12</t>
+  </si>
+  <si>
+    <t>2024-10-02</t>
   </si>
   <si>
     <t>harvest_amnt_12</t>
@@ -1598,175 +1601,175 @@
         <v>311</v>
       </c>
       <c r="DW1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="DX1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="DY1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="DZ1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="EA1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="EB1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="EC1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="ED1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="EE1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="EF1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="EG1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="EH1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="EI1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="EJ1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="EK1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="EL1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="EM1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="EN1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="EO1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="EP1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="EQ1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="ER1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="ES1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="ET1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="EU1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="EV1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="EW1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="EX1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="EY1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="EZ1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="FA1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="FB1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="FC1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="FD1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="FE1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="FF1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="FG1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="FH1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="FI1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="FJ1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="FK1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="FL1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="FM1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="FN1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="FO1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="FP1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="FQ1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="FR1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="FS1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="FT1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="FU1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="FV1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="FW1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="FX1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="FY1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="FZ1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="GA1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2">
@@ -2132,9 +2135,13 @@
       <c r="EP2" t="s">
         <v>77</v>
       </c>
-      <c r="EQ2" s="1"/>
+      <c r="EQ2" t="s">
+        <v>77</v>
+      </c>
       <c r="ER2" s="1"/>
-      <c r="ES2" s="1"/>
+      <c r="ES2" t="s">
+        <v>77</v>
+      </c>
       <c r="ET2" s="1"/>
       <c r="EU2" s="1"/>
       <c r="EV2" s="1"/>
@@ -2549,9 +2556,13 @@
       <c r="EP3" t="s">
         <v>77</v>
       </c>
-      <c r="EQ3" s="1"/>
+      <c r="EQ3" t="s">
+        <v>77</v>
+      </c>
       <c r="ER3" s="1"/>
-      <c r="ES3" s="1"/>
+      <c r="ES3" t="s">
+        <v>77</v>
+      </c>
       <c r="ET3" s="1"/>
       <c r="EU3" s="1"/>
       <c r="EV3" s="1"/>
@@ -2956,9 +2967,13 @@
       <c r="EP4" t="s">
         <v>77</v>
       </c>
-      <c r="EQ4" s="1"/>
+      <c r="EQ4" t="s">
+        <v>77</v>
+      </c>
       <c r="ER4" s="1"/>
-      <c r="ES4" s="1"/>
+      <c r="ES4" t="s">
+        <v>77</v>
+      </c>
       <c r="ET4" s="1"/>
       <c r="EU4" s="1"/>
       <c r="EV4" s="1"/>
@@ -3369,9 +3384,13 @@
       <c r="EP5" t="s">
         <v>77</v>
       </c>
-      <c r="EQ5" s="1"/>
+      <c r="EQ5" t="s">
+        <v>77</v>
+      </c>
       <c r="ER5" s="1"/>
-      <c r="ES5" s="1"/>
+      <c r="ES5" t="s">
+        <v>77</v>
+      </c>
       <c r="ET5" s="1"/>
       <c r="EU5" s="1"/>
       <c r="EV5" s="1"/>
@@ -3782,9 +3801,13 @@
       <c r="EP6" t="s">
         <v>77</v>
       </c>
-      <c r="EQ6" s="1"/>
+      <c r="EQ6" t="s">
+        <v>77</v>
+      </c>
       <c r="ER6" s="1"/>
-      <c r="ES6" s="1"/>
+      <c r="ES6" t="s">
+        <v>77</v>
+      </c>
       <c r="ET6" s="1"/>
       <c r="EU6" s="1"/>
       <c r="EV6" s="1"/>
@@ -4195,9 +4218,13 @@
       <c r="EP7" t="s">
         <v>77</v>
       </c>
-      <c r="EQ7" s="1"/>
+      <c r="EQ7" t="s">
+        <v>77</v>
+      </c>
       <c r="ER7" s="1"/>
-      <c r="ES7" s="1"/>
+      <c r="ES7" t="s">
+        <v>77</v>
+      </c>
       <c r="ET7" s="1"/>
       <c r="EU7" s="1"/>
       <c r="EV7" s="1"/>
@@ -4608,9 +4635,13 @@
       <c r="EP8" t="s">
         <v>77</v>
       </c>
-      <c r="EQ8" s="1"/>
+      <c r="EQ8" t="s">
+        <v>77</v>
+      </c>
       <c r="ER8" s="1"/>
-      <c r="ES8" s="1"/>
+      <c r="ES8" t="s">
+        <v>77</v>
+      </c>
       <c r="ET8" s="1"/>
       <c r="EU8" s="1"/>
       <c r="EV8" s="1"/>
@@ -5047,9 +5078,13 @@
       <c r="EP9" t="s">
         <v>77</v>
       </c>
-      <c r="EQ9" s="1"/>
+      <c r="EQ9" t="s">
+        <v>77</v>
+      </c>
       <c r="ER9" s="1"/>
-      <c r="ES9" s="1"/>
+      <c r="ES9" t="s">
+        <v>77</v>
+      </c>
       <c r="ET9" s="1"/>
       <c r="EU9" s="1"/>
       <c r="EV9" s="1"/>
@@ -5084,7 +5119,7 @@
       <c r="FY9" s="1"/>
       <c r="FZ9" s="1"/>
       <c r="GA9" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="10">
@@ -5480,9 +5515,13 @@
       <c r="EP10" t="s">
         <v>77</v>
       </c>
-      <c r="EQ10" s="1"/>
+      <c r="EQ10" t="s">
+        <v>77</v>
+      </c>
       <c r="ER10" s="1"/>
-      <c r="ES10" s="1"/>
+      <c r="ES10" t="s">
+        <v>77</v>
+      </c>
       <c r="ET10" s="1"/>
       <c r="EU10" s="1"/>
       <c r="EV10" s="1"/>
@@ -5517,7 +5556,7 @@
       <c r="FY10" s="1"/>
       <c r="FZ10" s="1"/>
       <c r="GA10" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11">
@@ -5897,9 +5936,13 @@
       <c r="EP11" t="s">
         <v>77</v>
       </c>
-      <c r="EQ11" s="1"/>
+      <c r="EQ11" t="s">
+        <v>77</v>
+      </c>
       <c r="ER11" s="1"/>
-      <c r="ES11" s="1"/>
+      <c r="ES11" t="s">
+        <v>77</v>
+      </c>
       <c r="ET11" s="1"/>
       <c r="EU11" s="1"/>
       <c r="EV11" s="1"/>
@@ -5934,7 +5977,7 @@
       <c r="FY11" s="1"/>
       <c r="FZ11" s="1"/>
       <c r="GA11" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12">
@@ -6340,9 +6383,13 @@
       <c r="EP12" t="s">
         <v>77</v>
       </c>
-      <c r="EQ12" s="1"/>
+      <c r="EQ12" t="s">
+        <v>77</v>
+      </c>
       <c r="ER12" s="1"/>
-      <c r="ES12" s="1"/>
+      <c r="ES12" t="s">
+        <v>77</v>
+      </c>
       <c r="ET12" s="1"/>
       <c r="EU12" s="1"/>
       <c r="EV12" s="1"/>
@@ -6377,7 +6424,7 @@
       <c r="FY12" s="1"/>
       <c r="FZ12" s="1"/>
       <c r="GA12" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13">
@@ -6785,9 +6832,13 @@
       <c r="EP13" t="s">
         <v>77</v>
       </c>
-      <c r="EQ13" s="1"/>
+      <c r="EQ13" t="s">
+        <v>77</v>
+      </c>
       <c r="ER13" s="1"/>
-      <c r="ES13" s="1"/>
+      <c r="ES13" t="s">
+        <v>77</v>
+      </c>
       <c r="ET13" s="1"/>
       <c r="EU13" s="1"/>
       <c r="EV13" s="1"/>
@@ -6822,7 +6873,7 @@
       <c r="FY13" s="1"/>
       <c r="FZ13" s="1"/>
       <c r="GA13" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14">
@@ -7228,9 +7279,13 @@
       <c r="EP14" t="s">
         <v>77</v>
       </c>
-      <c r="EQ14" s="1"/>
+      <c r="EQ14" t="s">
+        <v>77</v>
+      </c>
       <c r="ER14" s="1"/>
-      <c r="ES14" s="1"/>
+      <c r="ES14" t="s">
+        <v>77</v>
+      </c>
       <c r="ET14" s="1"/>
       <c r="EU14" s="1"/>
       <c r="EV14" s="1"/>
@@ -7265,7 +7320,7 @@
       <c r="FY14" s="1"/>
       <c r="FZ14" s="1"/>
       <c r="GA14" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15">
@@ -7661,9 +7716,13 @@
       <c r="EP15" t="s">
         <v>77</v>
       </c>
-      <c r="EQ15" s="1"/>
+      <c r="EQ15" t="s">
+        <v>77</v>
+      </c>
       <c r="ER15" s="1"/>
-      <c r="ES15" s="1"/>
+      <c r="ES15" t="s">
+        <v>77</v>
+      </c>
       <c r="ET15" s="1"/>
       <c r="EU15" s="1"/>
       <c r="EV15" s="1"/>
@@ -7698,7 +7757,7 @@
       <c r="FY15" s="1"/>
       <c r="FZ15" s="1"/>
       <c r="GA15" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="16">
@@ -8094,9 +8153,13 @@
       <c r="EP16" t="s">
         <v>77</v>
       </c>
-      <c r="EQ16" s="1"/>
+      <c r="EQ16" t="s">
+        <v>77</v>
+      </c>
       <c r="ER16" s="1"/>
-      <c r="ES16" s="1"/>
+      <c r="ES16" t="s">
+        <v>77</v>
+      </c>
       <c r="ET16" s="1"/>
       <c r="EU16" s="1"/>
       <c r="EV16" s="1"/>
@@ -8131,7 +8194,7 @@
       <c r="FY16" s="1"/>
       <c r="FZ16" s="1"/>
       <c r="GA16" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17">
@@ -8513,9 +8576,13 @@
       <c r="EP17" t="s">
         <v>77</v>
       </c>
-      <c r="EQ17" s="1"/>
+      <c r="EQ17" t="s">
+        <v>77</v>
+      </c>
       <c r="ER17" s="1"/>
-      <c r="ES17" s="1"/>
+      <c r="ES17" t="s">
+        <v>77</v>
+      </c>
       <c r="ET17" s="1"/>
       <c r="EU17" s="1"/>
       <c r="EV17" s="1"/>
@@ -8550,7 +8617,7 @@
       <c r="FY17" s="1"/>
       <c r="FZ17" s="1"/>
       <c r="GA17" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="18">
@@ -8932,9 +8999,13 @@
       <c r="EP18" t="s">
         <v>77</v>
       </c>
-      <c r="EQ18" s="1"/>
+      <c r="EQ18" t="s">
+        <v>77</v>
+      </c>
       <c r="ER18" s="1"/>
-      <c r="ES18" s="1"/>
+      <c r="ES18" t="s">
+        <v>77</v>
+      </c>
       <c r="ET18" s="1"/>
       <c r="EU18" s="1"/>
       <c r="EV18" s="1"/>
@@ -8969,7 +9040,7 @@
       <c r="FY18" s="1"/>
       <c r="FZ18" s="1"/>
       <c r="GA18" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19">
@@ -9351,9 +9422,13 @@
       <c r="EP19" t="s">
         <v>77</v>
       </c>
-      <c r="EQ19" s="1"/>
+      <c r="EQ19" t="s">
+        <v>77</v>
+      </c>
       <c r="ER19" s="1"/>
-      <c r="ES19" s="1"/>
+      <c r="ES19" t="s">
+        <v>77</v>
+      </c>
       <c r="ET19" s="1"/>
       <c r="EU19" s="1"/>
       <c r="EV19" s="1"/>
@@ -9388,7 +9463,7 @@
       <c r="FY19" s="1"/>
       <c r="FZ19" s="1"/>
       <c r="GA19" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20">
@@ -9770,9 +9845,13 @@
       <c r="EP20" t="s">
         <v>77</v>
       </c>
-      <c r="EQ20" s="1"/>
+      <c r="EQ20" t="s">
+        <v>77</v>
+      </c>
       <c r="ER20" s="1"/>
-      <c r="ES20" s="1"/>
+      <c r="ES20" t="s">
+        <v>77</v>
+      </c>
       <c r="ET20" s="1"/>
       <c r="EU20" s="1"/>
       <c r="EV20" s="1"/>
@@ -9807,7 +9886,7 @@
       <c r="FY20" s="1"/>
       <c r="FZ20" s="1"/>
       <c r="GA20" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="21">
@@ -10175,11 +10254,13 @@
         <v>267</v>
       </c>
       <c r="DV21" t="s">
-        <v>77</v>
-      </c>
-      <c r="DW21" s="1"/>
+        <v>312</v>
+      </c>
+      <c r="DW21" s="1">
+        <v>28</v>
+      </c>
       <c r="DX21" t="s">
-        <v>77</v>
+        <v>267</v>
       </c>
       <c r="DY21" t="s">
         <v>77</v>
@@ -10223,9 +10304,13 @@
       <c r="EP21" t="s">
         <v>77</v>
       </c>
-      <c r="EQ21" s="1"/>
+      <c r="EQ21" t="s">
+        <v>77</v>
+      </c>
       <c r="ER21" s="1"/>
-      <c r="ES21" s="1"/>
+      <c r="ES21" t="s">
+        <v>77</v>
+      </c>
       <c r="ET21" s="1"/>
       <c r="EU21" s="1"/>
       <c r="EV21" s="1"/>
@@ -10682,9 +10767,15 @@
       <c r="EP22" t="s">
         <v>267</v>
       </c>
-      <c r="EQ22" s="1"/>
-      <c r="ER22" s="1"/>
-      <c r="ES22" s="1"/>
+      <c r="EQ22" t="s">
+        <v>312</v>
+      </c>
+      <c r="ER22" s="1">
+        <v>19</v>
+      </c>
+      <c r="ES22" t="s">
+        <v>267</v>
+      </c>
       <c r="ET22" s="1"/>
       <c r="EU22" s="1"/>
       <c r="EV22" s="1"/>
@@ -11133,9 +11224,13 @@
       <c r="EP23" t="s">
         <v>77</v>
       </c>
-      <c r="EQ23" s="1"/>
+      <c r="EQ23" t="s">
+        <v>77</v>
+      </c>
       <c r="ER23" s="1"/>
-      <c r="ES23" s="1"/>
+      <c r="ES23" t="s">
+        <v>77</v>
+      </c>
       <c r="ET23" s="1"/>
       <c r="EU23" s="1"/>
       <c r="EV23" s="1"/>
@@ -11170,7 +11265,7 @@
       <c r="FY23" s="1"/>
       <c r="FZ23" s="1"/>
       <c r="GA23" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="24">
@@ -11578,9 +11673,13 @@
       <c r="EP24" t="s">
         <v>77</v>
       </c>
-      <c r="EQ24" s="1"/>
+      <c r="EQ24" t="s">
+        <v>77</v>
+      </c>
       <c r="ER24" s="1"/>
-      <c r="ES24" s="1"/>
+      <c r="ES24" t="s">
+        <v>77</v>
+      </c>
       <c r="ET24" s="1"/>
       <c r="EU24" s="1"/>
       <c r="EV24" s="1"/>
@@ -11997,9 +12096,13 @@
       <c r="EP25" t="s">
         <v>77</v>
       </c>
-      <c r="EQ25" s="1"/>
+      <c r="EQ25" t="s">
+        <v>77</v>
+      </c>
       <c r="ER25" s="1"/>
-      <c r="ES25" s="1"/>
+      <c r="ES25" t="s">
+        <v>77</v>
+      </c>
       <c r="ET25" s="1"/>
       <c r="EU25" s="1"/>
       <c r="EV25" s="1"/>
@@ -12412,9 +12515,13 @@
       <c r="EP26" t="s">
         <v>77</v>
       </c>
-      <c r="EQ26" s="1"/>
+      <c r="EQ26" t="s">
+        <v>77</v>
+      </c>
       <c r="ER26" s="1"/>
-      <c r="ES26" s="1"/>
+      <c r="ES26" t="s">
+        <v>77</v>
+      </c>
       <c r="ET26" s="1"/>
       <c r="EU26" s="1"/>
       <c r="EV26" s="1"/>
@@ -12449,7 +12556,7 @@
       <c r="FY26" s="1"/>
       <c r="FZ26" s="1"/>
       <c r="GA26" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="27">
@@ -12823,9 +12930,13 @@
       <c r="EP27" t="s">
         <v>77</v>
       </c>
-      <c r="EQ27" s="1"/>
+      <c r="EQ27" t="s">
+        <v>77</v>
+      </c>
       <c r="ER27" s="1"/>
-      <c r="ES27" s="1"/>
+      <c r="ES27" t="s">
+        <v>77</v>
+      </c>
       <c r="ET27" s="1"/>
       <c r="EU27" s="1"/>
       <c r="EV27" s="1"/>
@@ -13234,9 +13345,13 @@
       <c r="EP28" t="s">
         <v>77</v>
       </c>
-      <c r="EQ28" s="1"/>
+      <c r="EQ28" t="s">
+        <v>77</v>
+      </c>
       <c r="ER28" s="1"/>
-      <c r="ES28" s="1"/>
+      <c r="ES28" t="s">
+        <v>77</v>
+      </c>
       <c r="ET28" s="1"/>
       <c r="EU28" s="1"/>
       <c r="EV28" s="1"/>
@@ -13271,7 +13386,7 @@
       <c r="FY28" s="1"/>
       <c r="FZ28" s="1"/>
       <c r="GA28" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="29">
@@ -13645,9 +13760,13 @@
       <c r="EP29" t="s">
         <v>77</v>
       </c>
-      <c r="EQ29" s="1"/>
+      <c r="EQ29" t="s">
+        <v>77</v>
+      </c>
       <c r="ER29" s="1"/>
-      <c r="ES29" s="1"/>
+      <c r="ES29" t="s">
+        <v>77</v>
+      </c>
       <c r="ET29" s="1"/>
       <c r="EU29" s="1"/>
       <c r="EV29" s="1"/>
@@ -13682,7 +13801,7 @@
       <c r="FY29" s="1"/>
       <c r="FZ29" s="1"/>
       <c r="GA29" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="30">
@@ -14060,9 +14179,13 @@
       <c r="EP30" t="s">
         <v>77</v>
       </c>
-      <c r="EQ30" s="1"/>
+      <c r="EQ30" t="s">
+        <v>77</v>
+      </c>
       <c r="ER30" s="1"/>
-      <c r="ES30" s="1"/>
+      <c r="ES30" t="s">
+        <v>77</v>
+      </c>
       <c r="ET30" s="1"/>
       <c r="EU30" s="1"/>
       <c r="EV30" s="1"/>
@@ -14097,7 +14220,7 @@
       <c r="FY30" s="1"/>
       <c r="FZ30" s="1"/>
       <c r="GA30" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="31">
@@ -14475,9 +14598,13 @@
       <c r="EP31" t="s">
         <v>77</v>
       </c>
-      <c r="EQ31" s="1"/>
+      <c r="EQ31" t="s">
+        <v>77</v>
+      </c>
       <c r="ER31" s="1"/>
-      <c r="ES31" s="1"/>
+      <c r="ES31" t="s">
+        <v>77</v>
+      </c>
       <c r="ET31" s="1"/>
       <c r="EU31" s="1"/>
       <c r="EV31" s="1"/>
@@ -14512,7 +14639,7 @@
       <c r="FY31" s="1"/>
       <c r="FZ31" s="1"/>
       <c r="GA31" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="32">
@@ -14890,9 +15017,13 @@
       <c r="EP32" t="s">
         <v>77</v>
       </c>
-      <c r="EQ32" s="1"/>
+      <c r="EQ32" t="s">
+        <v>77</v>
+      </c>
       <c r="ER32" s="1"/>
-      <c r="ES32" s="1"/>
+      <c r="ES32" t="s">
+        <v>77</v>
+      </c>
       <c r="ET32" s="1"/>
       <c r="EU32" s="1"/>
       <c r="EV32" s="1"/>
@@ -14927,7 +15058,7 @@
       <c r="FY32" s="1"/>
       <c r="FZ32" s="1"/>
       <c r="GA32" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="33">
@@ -15305,9 +15436,13 @@
       <c r="EP33" t="s">
         <v>77</v>
       </c>
-      <c r="EQ33" s="1"/>
+      <c r="EQ33" t="s">
+        <v>77</v>
+      </c>
       <c r="ER33" s="1"/>
-      <c r="ES33" s="1"/>
+      <c r="ES33" t="s">
+        <v>77</v>
+      </c>
       <c r="ET33" s="1"/>
       <c r="EU33" s="1"/>
       <c r="EV33" s="1"/>
@@ -15342,7 +15477,7 @@
       <c r="FY33" s="1"/>
       <c r="FZ33" s="1"/>
       <c r="GA33" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="34">
@@ -15706,9 +15841,13 @@
       <c r="EP34" t="s">
         <v>77</v>
       </c>
-      <c r="EQ34" s="1"/>
+      <c r="EQ34" t="s">
+        <v>77</v>
+      </c>
       <c r="ER34" s="1"/>
-      <c r="ES34" s="1"/>
+      <c r="ES34" t="s">
+        <v>77</v>
+      </c>
       <c r="ET34" s="1"/>
       <c r="EU34" s="1"/>
       <c r="EV34" s="1"/>
@@ -15743,7 +15882,7 @@
       <c r="FY34" s="1"/>
       <c r="FZ34" s="1"/>
       <c r="GA34" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="35">
@@ -16107,9 +16246,13 @@
       <c r="EP35" t="s">
         <v>77</v>
       </c>
-      <c r="EQ35" s="1"/>
+      <c r="EQ35" t="s">
+        <v>77</v>
+      </c>
       <c r="ER35" s="1"/>
-      <c r="ES35" s="1"/>
+      <c r="ES35" t="s">
+        <v>77</v>
+      </c>
       <c r="ET35" s="1"/>
       <c r="EU35" s="1"/>
       <c r="EV35" s="1"/>
@@ -16144,7 +16287,7 @@
       <c r="FY35" s="1"/>
       <c r="FZ35" s="1"/>
       <c r="GA35" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="36">
@@ -16508,9 +16651,13 @@
       <c r="EP36" t="s">
         <v>77</v>
       </c>
-      <c r="EQ36" s="1"/>
+      <c r="EQ36" t="s">
+        <v>77</v>
+      </c>
       <c r="ER36" s="1"/>
-      <c r="ES36" s="1"/>
+      <c r="ES36" t="s">
+        <v>77</v>
+      </c>
       <c r="ET36" s="1"/>
       <c r="EU36" s="1"/>
       <c r="EV36" s="1"/>
@@ -16545,7 +16692,7 @@
       <c r="FY36" s="1"/>
       <c r="FZ36" s="1"/>
       <c r="GA36" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="37">
@@ -16909,9 +17056,13 @@
       <c r="EP37" t="s">
         <v>77</v>
       </c>
-      <c r="EQ37" s="1"/>
+      <c r="EQ37" t="s">
+        <v>77</v>
+      </c>
       <c r="ER37" s="1"/>
-      <c r="ES37" s="1"/>
+      <c r="ES37" t="s">
+        <v>77</v>
+      </c>
       <c r="ET37" s="1"/>
       <c r="EU37" s="1"/>
       <c r="EV37" s="1"/>
@@ -16946,7 +17097,7 @@
       <c r="FY37" s="1"/>
       <c r="FZ37" s="1"/>
       <c r="GA37" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="38">
@@ -17310,9 +17461,13 @@
       <c r="EP38" t="s">
         <v>77</v>
       </c>
-      <c r="EQ38" s="1"/>
+      <c r="EQ38" t="s">
+        <v>77</v>
+      </c>
       <c r="ER38" s="1"/>
-      <c r="ES38" s="1"/>
+      <c r="ES38" t="s">
+        <v>77</v>
+      </c>
       <c r="ET38" s="1"/>
       <c r="EU38" s="1"/>
       <c r="EV38" s="1"/>
@@ -17347,7 +17502,7 @@
       <c r="FY38" s="1"/>
       <c r="FZ38" s="1"/>
       <c r="GA38" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="39">
@@ -17713,9 +17868,13 @@
       <c r="EP39" t="s">
         <v>77</v>
       </c>
-      <c r="EQ39" s="1"/>
+      <c r="EQ39" t="s">
+        <v>77</v>
+      </c>
       <c r="ER39" s="1"/>
-      <c r="ES39" s="1"/>
+      <c r="ES39" t="s">
+        <v>77</v>
+      </c>
       <c r="ET39" s="1"/>
       <c r="EU39" s="1"/>
       <c r="EV39" s="1"/>
@@ -18116,9 +18275,13 @@
       <c r="EP40" t="s">
         <v>77</v>
       </c>
-      <c r="EQ40" s="1"/>
+      <c r="EQ40" t="s">
+        <v>77</v>
+      </c>
       <c r="ER40" s="1"/>
-      <c r="ES40" s="1"/>
+      <c r="ES40" t="s">
+        <v>77</v>
+      </c>
       <c r="ET40" s="1"/>
       <c r="EU40" s="1"/>
       <c r="EV40" s="1"/>
@@ -18519,9 +18682,13 @@
       <c r="EP41" t="s">
         <v>77</v>
       </c>
-      <c r="EQ41" s="1"/>
+      <c r="EQ41" t="s">
+        <v>77</v>
+      </c>
       <c r="ER41" s="1"/>
-      <c r="ES41" s="1"/>
+      <c r="ES41" t="s">
+        <v>77</v>
+      </c>
       <c r="ET41" s="1"/>
       <c r="EU41" s="1"/>
       <c r="EV41" s="1"/>
@@ -18922,9 +19089,13 @@
       <c r="EP42" t="s">
         <v>77</v>
       </c>
-      <c r="EQ42" s="1"/>
+      <c r="EQ42" t="s">
+        <v>77</v>
+      </c>
       <c r="ER42" s="1"/>
-      <c r="ES42" s="1"/>
+      <c r="ES42" t="s">
+        <v>77</v>
+      </c>
       <c r="ET42" s="1"/>
       <c r="EU42" s="1"/>
       <c r="EV42" s="1"/>
@@ -19325,9 +19496,13 @@
       <c r="EP43" t="s">
         <v>77</v>
       </c>
-      <c r="EQ43" s="1"/>
+      <c r="EQ43" t="s">
+        <v>77</v>
+      </c>
       <c r="ER43" s="1"/>
-      <c r="ES43" s="1"/>
+      <c r="ES43" t="s">
+        <v>77</v>
+      </c>
       <c r="ET43" s="1"/>
       <c r="EU43" s="1"/>
       <c r="EV43" s="1"/>
@@ -19730,9 +19905,13 @@
       <c r="EP44" t="s">
         <v>77</v>
       </c>
-      <c r="EQ44" s="1"/>
+      <c r="EQ44" t="s">
+        <v>77</v>
+      </c>
       <c r="ER44" s="1"/>
-      <c r="ES44" s="1"/>
+      <c r="ES44" t="s">
+        <v>77</v>
+      </c>
       <c r="ET44" s="1"/>
       <c r="EU44" s="1"/>
       <c r="EV44" s="1"/>
@@ -19767,7 +19946,7 @@
       <c r="FY44" s="1"/>
       <c r="FZ44" s="1"/>
       <c r="GA44" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="45">
@@ -20135,9 +20314,13 @@
       <c r="EP45" t="s">
         <v>77</v>
       </c>
-      <c r="EQ45" s="1"/>
+      <c r="EQ45" t="s">
+        <v>77</v>
+      </c>
       <c r="ER45" s="1"/>
-      <c r="ES45" s="1"/>
+      <c r="ES45" t="s">
+        <v>77</v>
+      </c>
       <c r="ET45" s="1"/>
       <c r="EU45" s="1"/>
       <c r="EV45" s="1"/>
@@ -20172,7 +20355,7 @@
       <c r="FY45" s="1"/>
       <c r="FZ45" s="1"/>
       <c r="GA45" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="46">
@@ -20542,9 +20725,13 @@
       <c r="EP46" t="s">
         <v>77</v>
       </c>
-      <c r="EQ46" s="1"/>
+      <c r="EQ46" t="s">
+        <v>77</v>
+      </c>
       <c r="ER46" s="1"/>
-      <c r="ES46" s="1"/>
+      <c r="ES46" t="s">
+        <v>77</v>
+      </c>
       <c r="ET46" s="1"/>
       <c r="EU46" s="1"/>
       <c r="EV46" s="1"/>
@@ -20579,7 +20766,7 @@
       <c r="FY46" s="1"/>
       <c r="FZ46" s="1"/>
       <c r="GA46" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="47">
@@ -20943,9 +21130,13 @@
       <c r="EP47" t="s">
         <v>77</v>
       </c>
-      <c r="EQ47" s="1"/>
+      <c r="EQ47" t="s">
+        <v>77</v>
+      </c>
       <c r="ER47" s="1"/>
-      <c r="ES47" s="1"/>
+      <c r="ES47" t="s">
+        <v>77</v>
+      </c>
       <c r="ET47" s="1"/>
       <c r="EU47" s="1"/>
       <c r="EV47" s="1"/>
@@ -20980,7 +21171,7 @@
       <c r="FY47" s="1"/>
       <c r="FZ47" s="1"/>
       <c r="GA47" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="48">
@@ -21354,9 +21545,13 @@
       <c r="EP48" t="s">
         <v>77</v>
       </c>
-      <c r="EQ48" s="1"/>
+      <c r="EQ48" t="s">
+        <v>77</v>
+      </c>
       <c r="ER48" s="1"/>
-      <c r="ES48" s="1"/>
+      <c r="ES48" t="s">
+        <v>77</v>
+      </c>
       <c r="ET48" s="1"/>
       <c r="EU48" s="1"/>
       <c r="EV48" s="1"/>
@@ -21391,7 +21586,7 @@
       <c r="FY48" s="1"/>
       <c r="FZ48" s="1"/>
       <c r="GA48" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="49">
@@ -21755,9 +21950,13 @@
       <c r="EP49" t="s">
         <v>77</v>
       </c>
-      <c r="EQ49" s="1"/>
+      <c r="EQ49" t="s">
+        <v>77</v>
+      </c>
       <c r="ER49" s="1"/>
-      <c r="ES49" s="1"/>
+      <c r="ES49" t="s">
+        <v>77</v>
+      </c>
       <c r="ET49" s="1"/>
       <c r="EU49" s="1"/>
       <c r="EV49" s="1"/>
@@ -21792,7 +21991,7 @@
       <c r="FY49" s="1"/>
       <c r="FZ49" s="1"/>
       <c r="GA49" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="50">
@@ -22156,9 +22355,13 @@
       <c r="EP50" t="s">
         <v>77</v>
       </c>
-      <c r="EQ50" s="1"/>
+      <c r="EQ50" t="s">
+        <v>77</v>
+      </c>
       <c r="ER50" s="1"/>
-      <c r="ES50" s="1"/>
+      <c r="ES50" t="s">
+        <v>77</v>
+      </c>
       <c r="ET50" s="1"/>
       <c r="EU50" s="1"/>
       <c r="EV50" s="1"/>
@@ -22193,7 +22396,7 @@
       <c r="FY50" s="1"/>
       <c r="FZ50" s="1"/>
       <c r="GA50" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="51">
@@ -22557,9 +22760,13 @@
       <c r="EP51" t="s">
         <v>77</v>
       </c>
-      <c r="EQ51" s="1"/>
+      <c r="EQ51" t="s">
+        <v>77</v>
+      </c>
       <c r="ER51" s="1"/>
-      <c r="ES51" s="1"/>
+      <c r="ES51" t="s">
+        <v>77</v>
+      </c>
       <c r="ET51" s="1"/>
       <c r="EU51" s="1"/>
       <c r="EV51" s="1"/>
@@ -22594,7 +22801,7 @@
       <c r="FY51" s="1"/>
       <c r="FZ51" s="1"/>
       <c r="GA51" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="52">
@@ -22958,9 +23165,13 @@
       <c r="EP52" t="s">
         <v>77</v>
       </c>
-      <c r="EQ52" s="1"/>
+      <c r="EQ52" t="s">
+        <v>77</v>
+      </c>
       <c r="ER52" s="1"/>
-      <c r="ES52" s="1"/>
+      <c r="ES52" t="s">
+        <v>77</v>
+      </c>
       <c r="ET52" s="1"/>
       <c r="EU52" s="1"/>
       <c r="EV52" s="1"/>
@@ -22995,7 +23206,7 @@
       <c r="FY52" s="1"/>
       <c r="FZ52" s="1"/>
       <c r="GA52" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="53">
@@ -23359,9 +23570,13 @@
       <c r="EP53" t="s">
         <v>77</v>
       </c>
-      <c r="EQ53" s="1"/>
+      <c r="EQ53" t="s">
+        <v>77</v>
+      </c>
       <c r="ER53" s="1"/>
-      <c r="ES53" s="1"/>
+      <c r="ES53" t="s">
+        <v>77</v>
+      </c>
       <c r="ET53" s="1"/>
       <c r="EU53" s="1"/>
       <c r="EV53" s="1"/>
@@ -23396,7 +23611,7 @@
       <c r="FY53" s="1"/>
       <c r="FZ53" s="1"/>
       <c r="GA53" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="54">
@@ -23760,9 +23975,13 @@
       <c r="EP54" t="s">
         <v>77</v>
       </c>
-      <c r="EQ54" s="1"/>
+      <c r="EQ54" t="s">
+        <v>77</v>
+      </c>
       <c r="ER54" s="1"/>
-      <c r="ES54" s="1"/>
+      <c r="ES54" t="s">
+        <v>77</v>
+      </c>
       <c r="ET54" s="1"/>
       <c r="EU54" s="1"/>
       <c r="EV54" s="1"/>
@@ -23797,7 +24016,7 @@
       <c r="FY54" s="1"/>
       <c r="FZ54" s="1"/>
       <c r="GA54" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="55">
@@ -24169,9 +24388,13 @@
       <c r="EP55" t="s">
         <v>77</v>
       </c>
-      <c r="EQ55" s="1"/>
+      <c r="EQ55" t="s">
+        <v>77</v>
+      </c>
       <c r="ER55" s="1"/>
-      <c r="ES55" s="1"/>
+      <c r="ES55" t="s">
+        <v>77</v>
+      </c>
       <c r="ET55" s="1"/>
       <c r="EU55" s="1"/>
       <c r="EV55" s="1"/>
@@ -24206,7 +24429,7 @@
       <c r="FY55" s="1"/>
       <c r="FZ55" s="1"/>
       <c r="GA55" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="56">
@@ -24582,9 +24805,13 @@
       <c r="EP56" t="s">
         <v>77</v>
       </c>
-      <c r="EQ56" s="1"/>
+      <c r="EQ56" t="s">
+        <v>77</v>
+      </c>
       <c r="ER56" s="1"/>
-      <c r="ES56" s="1"/>
+      <c r="ES56" t="s">
+        <v>77</v>
+      </c>
       <c r="ET56" s="1"/>
       <c r="EU56" s="1"/>
       <c r="EV56" s="1"/>
@@ -24619,7 +24846,7 @@
       <c r="FY56" s="1"/>
       <c r="FZ56" s="1"/>
       <c r="GA56" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="57">
@@ -24995,9 +25222,13 @@
       <c r="EP57" t="s">
         <v>77</v>
       </c>
-      <c r="EQ57" s="1"/>
+      <c r="EQ57" t="s">
+        <v>77</v>
+      </c>
       <c r="ER57" s="1"/>
-      <c r="ES57" s="1"/>
+      <c r="ES57" t="s">
+        <v>77</v>
+      </c>
       <c r="ET57" s="1"/>
       <c r="EU57" s="1"/>
       <c r="EV57" s="1"/>
@@ -25032,7 +25263,7 @@
       <c r="FY57" s="1"/>
       <c r="FZ57" s="1"/>
       <c r="GA57" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="58">
@@ -25404,9 +25635,13 @@
       <c r="EP58" t="s">
         <v>77</v>
       </c>
-      <c r="EQ58" s="1"/>
+      <c r="EQ58" t="s">
+        <v>77</v>
+      </c>
       <c r="ER58" s="1"/>
-      <c r="ES58" s="1"/>
+      <c r="ES58" t="s">
+        <v>77</v>
+      </c>
       <c r="ET58" s="1"/>
       <c r="EU58" s="1"/>
       <c r="EV58" s="1"/>
@@ -25813,9 +26048,13 @@
       <c r="EP59" t="s">
         <v>77</v>
       </c>
-      <c r="EQ59" s="1"/>
+      <c r="EQ59" t="s">
+        <v>77</v>
+      </c>
       <c r="ER59" s="1"/>
-      <c r="ES59" s="1"/>
+      <c r="ES59" t="s">
+        <v>77</v>
+      </c>
       <c r="ET59" s="1"/>
       <c r="EU59" s="1"/>
       <c r="EV59" s="1"/>
@@ -26224,9 +26463,13 @@
       <c r="EP60" t="s">
         <v>77</v>
       </c>
-      <c r="EQ60" s="1"/>
+      <c r="EQ60" t="s">
+        <v>77</v>
+      </c>
       <c r="ER60" s="1"/>
-      <c r="ES60" s="1"/>
+      <c r="ES60" t="s">
+        <v>77</v>
+      </c>
       <c r="ET60" s="1"/>
       <c r="EU60" s="1"/>
       <c r="EV60" s="1"/>
@@ -26261,7 +26504,7 @@
       <c r="FY60" s="1"/>
       <c r="FZ60" s="1"/>
       <c r="GA60" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="61">
@@ -26635,9 +26878,13 @@
       <c r="EP61" t="s">
         <v>77</v>
       </c>
-      <c r="EQ61" s="1"/>
+      <c r="EQ61" t="s">
+        <v>77</v>
+      </c>
       <c r="ER61" s="1"/>
-      <c r="ES61" s="1"/>
+      <c r="ES61" t="s">
+        <v>77</v>
+      </c>
       <c r="ET61" s="1"/>
       <c r="EU61" s="1"/>
       <c r="EV61" s="1"/>
@@ -26672,7 +26919,7 @@
       <c r="FY61" s="1"/>
       <c r="FZ61" s="1"/>
       <c r="GA61" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="62">
@@ -27036,9 +27283,13 @@
       <c r="EP62" t="s">
         <v>77</v>
       </c>
-      <c r="EQ62" s="1"/>
+      <c r="EQ62" t="s">
+        <v>77</v>
+      </c>
       <c r="ER62" s="1"/>
-      <c r="ES62" s="1"/>
+      <c r="ES62" t="s">
+        <v>77</v>
+      </c>
       <c r="ET62" s="1"/>
       <c r="EU62" s="1"/>
       <c r="EV62" s="1"/>
@@ -27437,9 +27688,13 @@
       <c r="EP63" t="s">
         <v>77</v>
       </c>
-      <c r="EQ63" s="1"/>
+      <c r="EQ63" t="s">
+        <v>77</v>
+      </c>
       <c r="ER63" s="1"/>
-      <c r="ES63" s="1"/>
+      <c r="ES63" t="s">
+        <v>77</v>
+      </c>
       <c r="ET63" s="1"/>
       <c r="EU63" s="1"/>
       <c r="EV63" s="1"/>
@@ -27838,9 +28093,13 @@
       <c r="EP64" t="s">
         <v>77</v>
       </c>
-      <c r="EQ64" s="1"/>
+      <c r="EQ64" t="s">
+        <v>77</v>
+      </c>
       <c r="ER64" s="1"/>
-      <c r="ES64" s="1"/>
+      <c r="ES64" t="s">
+        <v>77</v>
+      </c>
       <c r="ET64" s="1"/>
       <c r="EU64" s="1"/>
       <c r="EV64" s="1"/>
@@ -28243,9 +28502,13 @@
       <c r="EP65" t="s">
         <v>77</v>
       </c>
-      <c r="EQ65" s="1"/>
+      <c r="EQ65" t="s">
+        <v>77</v>
+      </c>
       <c r="ER65" s="1"/>
-      <c r="ES65" s="1"/>
+      <c r="ES65" t="s">
+        <v>77</v>
+      </c>
       <c r="ET65" s="1"/>
       <c r="EU65" s="1"/>
       <c r="EV65" s="1"/>
@@ -28280,7 +28543,7 @@
       <c r="FY65" s="1"/>
       <c r="FZ65" s="1"/>
       <c r="GA65" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="66">
@@ -28644,9 +28907,13 @@
       <c r="EP66" t="s">
         <v>77</v>
       </c>
-      <c r="EQ66" s="1"/>
+      <c r="EQ66" t="s">
+        <v>77</v>
+      </c>
       <c r="ER66" s="1"/>
-      <c r="ES66" s="1"/>
+      <c r="ES66" t="s">
+        <v>77</v>
+      </c>
       <c r="ET66" s="1"/>
       <c r="EU66" s="1"/>
       <c r="EV66" s="1"/>
@@ -28681,7 +28948,7 @@
       <c r="FY66" s="1"/>
       <c r="FZ66" s="1"/>
       <c r="GA66" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="67">
@@ -29055,9 +29322,13 @@
       <c r="EP67" t="s">
         <v>77</v>
       </c>
-      <c r="EQ67" s="1"/>
+      <c r="EQ67" t="s">
+        <v>77</v>
+      </c>
       <c r="ER67" s="1"/>
-      <c r="ES67" s="1"/>
+      <c r="ES67" t="s">
+        <v>77</v>
+      </c>
       <c r="ET67" s="1"/>
       <c r="EU67" s="1"/>
       <c r="EV67" s="1"/>
@@ -29092,7 +29363,7 @@
       <c r="FY67" s="1"/>
       <c r="FZ67" s="1"/>
       <c r="GA67" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="68">
@@ -29464,9 +29735,13 @@
       <c r="EP68" t="s">
         <v>77</v>
       </c>
-      <c r="EQ68" s="1"/>
+      <c r="EQ68" t="s">
+        <v>77</v>
+      </c>
       <c r="ER68" s="1"/>
-      <c r="ES68" s="1"/>
+      <c r="ES68" t="s">
+        <v>77</v>
+      </c>
       <c r="ET68" s="1"/>
       <c r="EU68" s="1"/>
       <c r="EV68" s="1"/>
@@ -29501,7 +29776,7 @@
       <c r="FY68" s="1"/>
       <c r="FZ68" s="1"/>
       <c r="GA68" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="69">
@@ -29873,9 +30148,13 @@
       <c r="EP69" t="s">
         <v>77</v>
       </c>
-      <c r="EQ69" s="1"/>
+      <c r="EQ69" t="s">
+        <v>77</v>
+      </c>
       <c r="ER69" s="1"/>
-      <c r="ES69" s="1"/>
+      <c r="ES69" t="s">
+        <v>77</v>
+      </c>
       <c r="ET69" s="1"/>
       <c r="EU69" s="1"/>
       <c r="EV69" s="1"/>
@@ -29910,7 +30189,7 @@
       <c r="FY69" s="1"/>
       <c r="FZ69" s="1"/>
       <c r="GA69" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="70">
@@ -30280,9 +30559,13 @@
       <c r="EP70" t="s">
         <v>77</v>
       </c>
-      <c r="EQ70" s="1"/>
+      <c r="EQ70" t="s">
+        <v>77</v>
+      </c>
       <c r="ER70" s="1"/>
-      <c r="ES70" s="1"/>
+      <c r="ES70" t="s">
+        <v>77</v>
+      </c>
       <c r="ET70" s="1"/>
       <c r="EU70" s="1"/>
       <c r="EV70" s="1"/>
@@ -30317,7 +30600,7 @@
       <c r="FY70" s="1"/>
       <c r="FZ70" s="1"/>
       <c r="GA70" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="71">
@@ -30687,9 +30970,13 @@
       <c r="EP71" t="s">
         <v>77</v>
       </c>
-      <c r="EQ71" s="1"/>
+      <c r="EQ71" t="s">
+        <v>77</v>
+      </c>
       <c r="ER71" s="1"/>
-      <c r="ES71" s="1"/>
+      <c r="ES71" t="s">
+        <v>77</v>
+      </c>
       <c r="ET71" s="1"/>
       <c r="EU71" s="1"/>
       <c r="EV71" s="1"/>
@@ -30724,7 +31011,7 @@
       <c r="FY71" s="1"/>
       <c r="FZ71" s="1"/>
       <c r="GA71" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="72">
@@ -31094,9 +31381,13 @@
       <c r="EP72" t="s">
         <v>77</v>
       </c>
-      <c r="EQ72" s="1"/>
+      <c r="EQ72" t="s">
+        <v>77</v>
+      </c>
       <c r="ER72" s="1"/>
-      <c r="ES72" s="1"/>
+      <c r="ES72" t="s">
+        <v>77</v>
+      </c>
       <c r="ET72" s="1"/>
       <c r="EU72" s="1"/>
       <c r="EV72" s="1"/>
@@ -31501,9 +31792,13 @@
       <c r="EP73" t="s">
         <v>77</v>
       </c>
-      <c r="EQ73" s="1"/>
+      <c r="EQ73" t="s">
+        <v>77</v>
+      </c>
       <c r="ER73" s="1"/>
-      <c r="ES73" s="1"/>
+      <c r="ES73" t="s">
+        <v>77</v>
+      </c>
       <c r="ET73" s="1"/>
       <c r="EU73" s="1"/>
       <c r="EV73" s="1"/>
@@ -31904,9 +32199,13 @@
       <c r="EP74" t="s">
         <v>77</v>
       </c>
-      <c r="EQ74" s="1"/>
+      <c r="EQ74" t="s">
+        <v>77</v>
+      </c>
       <c r="ER74" s="1"/>
-      <c r="ES74" s="1"/>
+      <c r="ES74" t="s">
+        <v>77</v>
+      </c>
       <c r="ET74" s="1"/>
       <c r="EU74" s="1"/>
       <c r="EV74" s="1"/>
@@ -32307,9 +32606,13 @@
       <c r="EP75" t="s">
         <v>77</v>
       </c>
-      <c r="EQ75" s="1"/>
+      <c r="EQ75" t="s">
+        <v>77</v>
+      </c>
       <c r="ER75" s="1"/>
-      <c r="ES75" s="1"/>
+      <c r="ES75" t="s">
+        <v>77</v>
+      </c>
       <c r="ET75" s="1"/>
       <c r="EU75" s="1"/>
       <c r="EV75" s="1"/>

</xml_diff>

<commit_message>
2024 crop & sales data indicators
</commit_message>
<xml_diff>
--- a/analytics/modified_data/tbf_market_garden_data_2024_clean.xlsx
+++ b/analytics/modified_data/tbf_market_garden_data_2024_clean.xlsx
@@ -32518,7 +32518,7 @@
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K48" s="2">
         <v>50</v>
@@ -36859,7 +36859,7 @@
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K55" s="2">
         <v>50</v>
@@ -37494,7 +37494,7 @@
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K56" s="2">
         <v>75</v>
@@ -38137,7 +38137,7 @@
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K57" s="2">
         <v>75</v>
@@ -43179,7 +43179,7 @@
       </c>
       <c r="I65" s="2"/>
       <c r="J65" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K65" s="2">
         <v>50</v>
@@ -43806,7 +43806,7 @@
       </c>
       <c r="I66" s="2"/>
       <c r="J66" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K66" s="2">
         <v>46</v>
@@ -46328,7 +46328,7 @@
       </c>
       <c r="I70" s="2"/>
       <c r="J70" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K70" s="2">
         <v>40</v>
@@ -46957,7 +46957,7 @@
       </c>
       <c r="I71" s="2"/>
       <c r="J71" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K71" s="2">
         <v>40</v>

</xml_diff>